<commit_message>
SVM Dataset Completo normalizado e nao normalizado e PCA
</commit_message>
<xml_diff>
--- a/model_results/all_models_results.xlsx
+++ b/model_results/all_models_results.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Mestrado\projeto_SIN5007_rec_padroes\model_results\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433AA175-077D-416F-A90E-8F0B1D5DA865}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="6885" windowWidth="25770" windowHeight="8820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="20">
   <si>
     <t>Atividade</t>
   </si>
@@ -31,17 +25,62 @@
     <t>Condicao</t>
   </si>
   <si>
+    <t>Melhores_Params</t>
+  </si>
+  <si>
     <t>Metrica</t>
   </si>
   <si>
     <t>Valor</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>SVC</t>
+  </si>
+  <si>
+    <t>Dataset Completo Desbalanceado - Nao Normalizado</t>
+  </si>
+  <si>
+    <t>Dataset Completo Balanceado - Nao Normalizado</t>
+  </si>
+  <si>
+    <t>Dataset Completo Desbalanceado - Normalizado</t>
+  </si>
+  <si>
+    <t>Dataset Completo Balanceado - Normalizado</t>
+  </si>
+  <si>
+    <t>PCA Desbalanceado</t>
+  </si>
+  <si>
+    <t>PCA Balanceado</t>
+  </si>
+  <si>
+    <t>('linear', 1, 'scale')</t>
+  </si>
+  <si>
+    <t>('rbf', 100, '0.0001')</t>
+  </si>
+  <si>
+    <t>('sigmoid', 1, '0.0001')</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>Precision</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,19 +143,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -158,7 +189,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -190,27 +221,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -242,24 +255,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -435,16 +430,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -459,6 +452,369 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2">
+        <v>0.9603830369357045</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4">
+        <v>0.677579365079365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5">
+        <v>0.9627086183310534</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <v>0.8766666666666666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7">
+        <v>0.6900793650793651</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8">
+        <v>0.9627086183310534</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9">
+        <v>0.8766666666666666</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10">
+        <v>0.6900793650793651</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11">
+        <v>0.9591928864569083</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12">
+        <v>0.9100000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13">
+        <v>0.6730158730158731</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14">
+        <v>0.9638987688098494</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15">
+        <v>0.6399999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16">
+        <v>0.7995238095238095</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17">
+        <v>0.9580574555403556</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18">
+        <v>0.7166666666666666</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19">
+        <v>0.7138095238095238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Naive Bayes armazenando valores
</commit_message>
<xml_diff>
--- a/model_results/all_models_results.xlsx
+++ b/model_results/all_models_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="27">
   <si>
     <t>Atividade</t>
   </si>
@@ -34,12 +34,15 @@
     <t>Valor</t>
   </si>
   <si>
-    <t>7</t>
+    <t>6</t>
   </si>
   <si>
     <t>SVC</t>
   </si>
   <si>
+    <t>Naive Bayes</t>
+  </si>
+  <si>
     <t>Dataset Completo Desbalanceado - Nao Normalizado</t>
   </si>
   <si>
@@ -56,6 +59,24 @@
   </si>
   <si>
     <t>PCA Balanceado</t>
+  </si>
+  <si>
+    <t>Branch and Bound Desbalanceado</t>
+  </si>
+  <si>
+    <t>Branch and Bound Balanceado</t>
+  </si>
+  <si>
+    <t>Dataset Completo Desbalanceado</t>
+  </si>
+  <si>
+    <t>Dataset Completo Balanceado</t>
+  </si>
+  <si>
+    <t>ReliefF Desbalanceado</t>
+  </si>
+  <si>
+    <t>ReliefF Balanceado</t>
   </si>
   <si>
     <t>('linear', 1, 'scale')</t>
@@ -431,7 +452,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -465,13 +486,13 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F2">
         <v>0.9603830369357045</v>
@@ -485,13 +506,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F3">
         <v>0.86</v>
@@ -505,13 +526,13 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F4">
         <v>0.677579365079365</v>
@@ -525,13 +546,13 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F5">
         <v>0.9627086183310534</v>
@@ -545,13 +566,13 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F6">
         <v>0.8766666666666666</v>
@@ -565,13 +586,13 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F7">
         <v>0.6900793650793651</v>
@@ -585,13 +606,13 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F8">
         <v>0.9627086183310534</v>
@@ -605,13 +626,13 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F9">
         <v>0.8766666666666666</v>
@@ -625,13 +646,13 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F10">
         <v>0.6900793650793651</v>
@@ -645,13 +666,13 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F11">
         <v>0.9591928864569083</v>
@@ -665,13 +686,13 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F12">
         <v>0.9100000000000001</v>
@@ -685,136 +706,616 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F13">
         <v>0.6730158730158731</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>6</v>
+      <c r="A14">
+        <v>7</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F14">
         <v>0.9638987688098494</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>6</v>
+      <c r="A15">
+        <v>7</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F15">
         <v>0.6399999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>6</v>
+      <c r="A16">
+        <v>7</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F16">
         <v>0.7995238095238095</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>6</v>
+      <c r="A17">
+        <v>7</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F17">
         <v>0.9580574555403556</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>6</v>
+      <c r="A18">
+        <v>7</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F18">
         <v>0.7166666666666666</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>6</v>
+      <c r="A19">
+        <v>7</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E19" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F19">
         <v>0.7138095238095238</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20">
+        <v>0.6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20">
+        <v>0.9312448700410396</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21">
+        <v>0.6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22">
+        <v>0.6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23">
+        <v>0.3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23">
+        <v>0.6901094391244869</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24">
+        <v>0.3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24">
+        <v>0.2166666666666667</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25">
+        <v>0.3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25">
+        <v>0.04927119294207902</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26">
+        <v>0.6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26">
+        <v>0.9556771545827634</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27">
+        <v>0.6</v>
+      </c>
+      <c r="E27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27">
+        <v>0.7166666666666666</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28">
+        <v>0.6</v>
+      </c>
+      <c r="E28" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28">
+        <v>0.6753968253968254</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29">
+        <v>0.8</v>
+      </c>
+      <c r="E29" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29">
+        <v>0.9393296853625172</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30">
+        <v>0.8</v>
+      </c>
+      <c r="E30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30">
+        <v>0.8766666666666666</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31">
+        <v>0.8</v>
+      </c>
+      <c r="E31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31">
+        <v>0.547142857142857</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32">
+        <v>0.9335567715458277</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>26</v>
+      </c>
+      <c r="F34">
+        <v>0.2166666666666666</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <v>6</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35">
+        <v>0.9416963064295485</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36">
+        <v>6</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37">
+        <v>0.5704761904761905</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38">
+        <v>0.4</v>
+      </c>
+      <c r="E38" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38">
+        <v>0.9627222982216141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39">
+        <v>0.4</v>
+      </c>
+      <c r="E39" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39">
+        <v>0.6966666666666667</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40">
+        <v>0.4</v>
+      </c>
+      <c r="E40" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40">
+        <v>0.7538095238095239</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41">
+        <v>0.1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F41">
+        <v>0.9568946648426813</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42">
+        <v>0.1</v>
+      </c>
+      <c r="E42" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42">
+        <v>0.8766666666666666</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43">
+        <v>0.1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>26</v>
+      </c>
+      <c r="F43">
+        <v>0.6523015873015873</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SVM com Branch and Bound
</commit_message>
<xml_diff>
--- a/model_results/all_models_results.xlsx
+++ b/model_results/all_models_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="31">
   <si>
     <t>Atividade</t>
   </si>
@@ -34,7 +34,7 @@
     <t>Valor</t>
   </si>
   <si>
-    <t>6</t>
+    <t>7</t>
   </si>
   <si>
     <t>SVC</t>
@@ -79,6 +79,12 @@
     <t>ReliefF Balanceado</t>
   </si>
   <si>
+    <t>Branch and Bound - Sem Normalização - Desbalanceado</t>
+  </si>
+  <si>
+    <t>Branch and Bound - Sem Normalização - Balanceado</t>
+  </si>
+  <si>
     <t>('linear', 1, 'scale')</t>
   </si>
   <si>
@@ -86,6 +92,12 @@
   </si>
   <si>
     <t>('sigmoid', 1, '0.0001')</t>
+  </si>
+  <si>
+    <t>('rbf', 10, '0.9201')</t>
+  </si>
+  <si>
+    <t>('sigmoid', 1, '0.0201')</t>
   </si>
   <si>
     <t>Accuracy</t>
@@ -452,7 +464,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -489,10 +501,10 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F2">
         <v>0.9603830369357045</v>
@@ -509,10 +521,10 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F3">
         <v>0.86</v>
@@ -529,10 +541,10 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F4">
         <v>0.677579365079365</v>
@@ -549,10 +561,10 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F5">
         <v>0.9627086183310534</v>
@@ -569,10 +581,10 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F6">
         <v>0.8766666666666666</v>
@@ -589,10 +601,10 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F7">
         <v>0.6900793650793651</v>
@@ -609,10 +621,10 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F8">
         <v>0.9627086183310534</v>
@@ -629,10 +641,10 @@
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F9">
         <v>0.8766666666666666</v>
@@ -649,10 +661,10 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F10">
         <v>0.6900793650793651</v>
@@ -669,10 +681,10 @@
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F11">
         <v>0.9591928864569083</v>
@@ -689,10 +701,10 @@
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F12">
         <v>0.9100000000000001</v>
@@ -709,10 +721,10 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F13">
         <v>0.6730158730158731</v>
@@ -729,10 +741,10 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E14" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F14">
         <v>0.9638987688098494</v>
@@ -749,10 +761,10 @@
         <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F15">
         <v>0.6399999999999999</v>
@@ -769,10 +781,10 @@
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F16">
         <v>0.7995238095238095</v>
@@ -789,10 +801,10 @@
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F17">
         <v>0.9580574555403556</v>
@@ -809,10 +821,10 @@
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F18">
         <v>0.7166666666666666</v>
@@ -829,10 +841,10 @@
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F19">
         <v>0.7138095238095238</v>
@@ -852,7 +864,7 @@
         <v>0.6</v>
       </c>
       <c r="E20" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F20">
         <v>0.9312448700410396</v>
@@ -872,7 +884,7 @@
         <v>0.6</v>
       </c>
       <c r="E21" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -892,7 +904,7 @@
         <v>0.6</v>
       </c>
       <c r="E22" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -912,7 +924,7 @@
         <v>0.3</v>
       </c>
       <c r="E23" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F23">
         <v>0.6901094391244869</v>
@@ -932,7 +944,7 @@
         <v>0.3</v>
       </c>
       <c r="E24" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F24">
         <v>0.2166666666666667</v>
@@ -952,7 +964,7 @@
         <v>0.3</v>
       </c>
       <c r="E25" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F25">
         <v>0.04927119294207902</v>
@@ -972,7 +984,7 @@
         <v>0.6</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F26">
         <v>0.9556771545827634</v>
@@ -992,7 +1004,7 @@
         <v>0.6</v>
       </c>
       <c r="E27" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F27">
         <v>0.7166666666666666</v>
@@ -1012,7 +1024,7 @@
         <v>0.6</v>
       </c>
       <c r="E28" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F28">
         <v>0.6753968253968254</v>
@@ -1032,7 +1044,7 @@
         <v>0.8</v>
       </c>
       <c r="E29" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F29">
         <v>0.9393296853625172</v>
@@ -1052,7 +1064,7 @@
         <v>0.8</v>
       </c>
       <c r="E30" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F30">
         <v>0.8766666666666666</v>
@@ -1072,7 +1084,7 @@
         <v>0.8</v>
       </c>
       <c r="E31" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F31">
         <v>0.547142857142857</v>
@@ -1092,7 +1104,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F32">
         <v>0.9335567715458277</v>
@@ -1112,7 +1124,7 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F33">
         <v>0.11</v>
@@ -1132,7 +1144,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F34">
         <v>0.2166666666666666</v>
@@ -1152,7 +1164,7 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F35">
         <v>0.9416963064295485</v>
@@ -1172,7 +1184,7 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F36">
         <v>0.64</v>
@@ -1192,14 +1204,14 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F37">
         <v>0.5704761904761905</v>
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" t="s">
+      <c r="A38">
         <v>6</v>
       </c>
       <c r="B38" t="s">
@@ -1212,14 +1224,14 @@
         <v>0.4</v>
       </c>
       <c r="E38" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F38">
         <v>0.9627222982216141</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" t="s">
+      <c r="A39">
         <v>6</v>
       </c>
       <c r="B39" t="s">
@@ -1232,14 +1244,14 @@
         <v>0.4</v>
       </c>
       <c r="E39" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F39">
         <v>0.6966666666666667</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" t="s">
+      <c r="A40">
         <v>6</v>
       </c>
       <c r="B40" t="s">
@@ -1252,14 +1264,14 @@
         <v>0.4</v>
       </c>
       <c r="E40" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F40">
         <v>0.7538095238095239</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" t="s">
+      <c r="A41">
         <v>6</v>
       </c>
       <c r="B41" t="s">
@@ -1272,14 +1284,14 @@
         <v>0.1</v>
       </c>
       <c r="E41" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F41">
         <v>0.9568946648426813</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" t="s">
+      <c r="A42">
         <v>6</v>
       </c>
       <c r="B42" t="s">
@@ -1292,14 +1304,14 @@
         <v>0.1</v>
       </c>
       <c r="E42" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F42">
         <v>0.8766666666666666</v>
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" t="s">
+      <c r="A43">
         <v>6</v>
       </c>
       <c r="B43" t="s">
@@ -1312,10 +1324,130 @@
         <v>0.1</v>
       </c>
       <c r="E43" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F43">
         <v>0.6523015873015873</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" t="s">
+        <v>26</v>
+      </c>
+      <c r="E44" t="s">
+        <v>28</v>
+      </c>
+      <c r="F44">
+        <v>0.9382352941176469</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" t="s">
+        <v>29</v>
+      </c>
+      <c r="F45">
+        <v>0.08333333333333333</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" t="s">
+        <v>26</v>
+      </c>
+      <c r="E46" t="s">
+        <v>30</v>
+      </c>
+      <c r="F46">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" t="s">
+        <v>28</v>
+      </c>
+      <c r="F47">
+        <v>0.8961285909712722</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D48" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48" t="s">
+        <v>29</v>
+      </c>
+      <c r="F48">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" t="s">
+        <v>30</v>
+      </c>
+      <c r="F49">
+        <v>0.006666666666666668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Naive Bayes normalizado e nao normalizado
</commit_message>
<xml_diff>
--- a/model_results/all_models_results.xlsx
+++ b/model_results/all_models_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="33">
   <si>
     <t>Atividade</t>
   </si>
@@ -34,7 +34,7 @@
     <t>Valor</t>
   </si>
   <si>
-    <t>7</t>
+    <t>6</t>
   </si>
   <si>
     <t>SVC</t>
@@ -61,28 +61,34 @@
     <t>PCA Balanceado</t>
   </si>
   <si>
-    <t>Branch and Bound Desbalanceado</t>
-  </si>
-  <si>
-    <t>Branch and Bound Balanceado</t>
-  </si>
-  <si>
-    <t>Dataset Completo Desbalanceado</t>
-  </si>
-  <si>
-    <t>Dataset Completo Balanceado</t>
-  </si>
-  <si>
-    <t>ReliefF Desbalanceado</t>
-  </si>
-  <si>
-    <t>ReliefF Balanceado</t>
-  </si>
-  <si>
     <t>Branch and Bound - Sem Normalização - Desbalanceado</t>
   </si>
   <si>
     <t>Branch and Bound - Sem Normalização - Balanceado</t>
+  </si>
+  <si>
+    <t>Branch and Bound Desbalanceado - Nao Normalizado</t>
+  </si>
+  <si>
+    <t>Branch and Bound Balanceado - Nao Normalizado</t>
+  </si>
+  <si>
+    <t>ReliefF Desbalanceado - Nao Normalizado</t>
+  </si>
+  <si>
+    <t>ReliefF Balanceado - Nao Normalizado</t>
+  </si>
+  <si>
+    <t>ReliefF Desbalanceado - Normalizado</t>
+  </si>
+  <si>
+    <t>ReliefF Balanceado - Normalizado</t>
+  </si>
+  <si>
+    <t>Branch and Bound Desbalanceado - Normalizado</t>
+  </si>
+  <si>
+    <t>Branch and Bound Balanceado - Normalizado</t>
   </si>
   <si>
     <t>('linear', 1, 'scale')</t>
@@ -464,7 +470,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -501,10 +507,10 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F2">
         <v>0.9603830369357045</v>
@@ -521,10 +527,10 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F3">
         <v>0.86</v>
@@ -541,10 +547,10 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F4">
         <v>0.677579365079365</v>
@@ -561,10 +567,10 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F5">
         <v>0.9627086183310534</v>
@@ -581,10 +587,10 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F6">
         <v>0.8766666666666666</v>
@@ -601,10 +607,10 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F7">
         <v>0.6900793650793651</v>
@@ -621,10 +627,10 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F8">
         <v>0.9627086183310534</v>
@@ -641,10 +647,10 @@
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F9">
         <v>0.8766666666666666</v>
@@ -661,10 +667,10 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F10">
         <v>0.6900793650793651</v>
@@ -681,10 +687,10 @@
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F11">
         <v>0.9591928864569083</v>
@@ -701,10 +707,10 @@
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F12">
         <v>0.9100000000000001</v>
@@ -721,10 +727,10 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F13">
         <v>0.6730158730158731</v>
@@ -741,10 +747,10 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F14">
         <v>0.9638987688098494</v>
@@ -761,10 +767,10 @@
         <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F15">
         <v>0.6399999999999999</v>
@@ -781,10 +787,10 @@
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F16">
         <v>0.7995238095238095</v>
@@ -801,10 +807,10 @@
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F17">
         <v>0.9580574555403556</v>
@@ -821,10 +827,10 @@
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E18" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F18">
         <v>0.7166666666666666</v>
@@ -841,10 +847,10 @@
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F19">
         <v>0.7138095238095238</v>
@@ -852,122 +858,122 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
         <v>15</v>
       </c>
-      <c r="D20">
-        <v>0.6</v>
+      <c r="D20" t="s">
+        <v>28</v>
       </c>
       <c r="E20" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F20">
-        <v>0.9312448700410396</v>
+        <v>0.9382352941176469</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21" t="s">
         <v>15</v>
       </c>
-      <c r="D21">
-        <v>0.6</v>
+      <c r="D21" t="s">
+        <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>0.08333333333333333</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
         <v>15</v>
       </c>
-      <c r="D22">
-        <v>0.6</v>
+      <c r="D22" t="s">
+        <v>28</v>
       </c>
       <c r="E22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
         <v>16</v>
       </c>
-      <c r="D23">
-        <v>0.3</v>
+      <c r="D23" t="s">
+        <v>29</v>
       </c>
       <c r="E23" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F23">
-        <v>0.6901094391244869</v>
+        <v>0.8961285909712722</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
         <v>16</v>
       </c>
-      <c r="D24">
-        <v>0.3</v>
+      <c r="D24" t="s">
+        <v>29</v>
       </c>
       <c r="E24" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F24">
-        <v>0.2166666666666667</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
         <v>16</v>
       </c>
-      <c r="D25">
-        <v>0.3</v>
+      <c r="D25" t="s">
+        <v>29</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F25">
-        <v>0.04927119294207902</v>
+        <v>0.006666666666666668</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -984,10 +990,10 @@
         <v>0.6</v>
       </c>
       <c r="E26" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F26">
-        <v>0.9556771545827634</v>
+        <v>0.9312448700410396</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1004,10 +1010,10 @@
         <v>0.6</v>
       </c>
       <c r="E27" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F27">
-        <v>0.7166666666666666</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1024,10 +1030,10 @@
         <v>0.6</v>
       </c>
       <c r="E28" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F28">
-        <v>0.6753968253968254</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1041,13 +1047,13 @@
         <v>18</v>
       </c>
       <c r="D29">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="E29" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F29">
-        <v>0.9393296853625172</v>
+        <v>0.6901094391244869</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1061,13 +1067,13 @@
         <v>18</v>
       </c>
       <c r="D30">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="E30" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F30">
-        <v>0.8766666666666666</v>
+        <v>0.2166666666666667</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1081,13 +1087,13 @@
         <v>18</v>
       </c>
       <c r="D31">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="E31" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F31">
-        <v>0.547142857142857</v>
+        <v>0.04927119294207902</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1101,10 +1107,10 @@
         <v>13</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E32" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F32">
         <v>0.9335567715458277</v>
@@ -1121,10 +1127,10 @@
         <v>13</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E33" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F33">
         <v>0.11</v>
@@ -1141,10 +1147,10 @@
         <v>13</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E34" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F34">
         <v>0.2166666666666666</v>
@@ -1164,10 +1170,10 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F35">
-        <v>0.9416963064295485</v>
+        <v>0.9428590971272228</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1184,7 +1190,7 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F36">
         <v>0.64</v>
@@ -1204,10 +1210,10 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F37">
-        <v>0.5704761904761905</v>
+        <v>0.5904761904761904</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1224,7 +1230,7 @@
         <v>0.4</v>
       </c>
       <c r="E38" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F38">
         <v>0.9627222982216141</v>
@@ -1244,7 +1250,7 @@
         <v>0.4</v>
       </c>
       <c r="E39" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F39">
         <v>0.6966666666666667</v>
@@ -1264,7 +1270,7 @@
         <v>0.4</v>
       </c>
       <c r="E40" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F40">
         <v>0.7538095238095239</v>
@@ -1284,7 +1290,7 @@
         <v>0.1</v>
       </c>
       <c r="E41" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F41">
         <v>0.9568946648426813</v>
@@ -1304,7 +1310,7 @@
         <v>0.1</v>
       </c>
       <c r="E42" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F42">
         <v>0.8766666666666666</v>
@@ -1324,130 +1330,490 @@
         <v>0.1</v>
       </c>
       <c r="E43" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F43">
         <v>0.6523015873015873</v>
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" t="s">
+      <c r="A44">
         <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44">
+        <v>0.6</v>
+      </c>
+      <c r="E44" t="s">
+        <v>30</v>
+      </c>
+      <c r="F44">
+        <v>0.9556771545827634</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45">
+        <v>6</v>
+      </c>
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45">
+        <v>0.6</v>
+      </c>
+      <c r="E45" t="s">
+        <v>31</v>
+      </c>
+      <c r="F45">
+        <v>0.7166666666666666</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46">
+        <v>6</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46">
+        <v>0.6</v>
+      </c>
+      <c r="E46" t="s">
+        <v>32</v>
+      </c>
+      <c r="F46">
+        <v>0.6753968253968254</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47">
+        <v>6</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47">
+        <v>0.8</v>
+      </c>
+      <c r="E47" t="s">
+        <v>30</v>
+      </c>
+      <c r="F47">
+        <v>0.9393296853625172</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48">
+        <v>6</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48">
+        <v>0.8</v>
+      </c>
+      <c r="E48" t="s">
+        <v>31</v>
+      </c>
+      <c r="F48">
+        <v>0.8766666666666666</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49">
+        <v>6</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49">
+        <v>0.8</v>
+      </c>
+      <c r="E49" t="s">
+        <v>32</v>
+      </c>
+      <c r="F49">
+        <v>0.547142857142857</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50">
+        <v>6</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50">
+        <v>0.9</v>
+      </c>
+      <c r="E50" t="s">
+        <v>30</v>
+      </c>
+      <c r="F50">
+        <v>0.9475376196990425</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51">
+        <v>6</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51">
+        <v>0.9</v>
+      </c>
+      <c r="E51" t="s">
+        <v>31</v>
+      </c>
+      <c r="F51">
+        <v>0.7166666666666666</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52">
+        <v>6</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52">
+        <v>0.9</v>
+      </c>
+      <c r="E52" t="s">
+        <v>32</v>
+      </c>
+      <c r="F52">
+        <v>0.6044444444444445</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53">
+        <v>6</v>
+      </c>
+      <c r="B53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53">
+        <v>0.2</v>
+      </c>
+      <c r="E53" t="s">
+        <v>30</v>
+      </c>
+      <c r="F53">
+        <v>0.9358413132694938</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54">
+        <v>6</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54">
+        <v>0.2</v>
+      </c>
+      <c r="E54" t="s">
+        <v>31</v>
+      </c>
+      <c r="F54">
+        <v>0.8766666666666666</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55">
+        <v>6</v>
+      </c>
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55">
+        <v>0.2</v>
+      </c>
+      <c r="E55" t="s">
+        <v>32</v>
+      </c>
+      <c r="F55">
+        <v>0.5276984126984127</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56">
+        <v>6</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" t="s">
         <v>21</v>
       </c>
-      <c r="D44" t="s">
-        <v>26</v>
-      </c>
-      <c r="E44" t="s">
-        <v>28</v>
-      </c>
-      <c r="F44">
-        <v>0.9382352941176469</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" t="s">
-        <v>6</v>
-      </c>
-      <c r="B45" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="D56">
+        <v>0.8</v>
+      </c>
+      <c r="E56" t="s">
+        <v>30</v>
+      </c>
+      <c r="F56">
+        <v>0.9627222982216141</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57">
+        <v>6</v>
+      </c>
+      <c r="B57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" t="s">
         <v>21</v>
       </c>
-      <c r="D45" t="s">
-        <v>26</v>
-      </c>
-      <c r="E45" t="s">
-        <v>29</v>
-      </c>
-      <c r="F45">
-        <v>0.08333333333333333</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" t="s">
-        <v>6</v>
-      </c>
-      <c r="B46" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="D57">
+        <v>0.8</v>
+      </c>
+      <c r="E57" t="s">
+        <v>31</v>
+      </c>
+      <c r="F57">
+        <v>0.6966666666666667</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58">
+        <v>6</v>
+      </c>
+      <c r="B58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" t="s">
         <v>21</v>
       </c>
-      <c r="D46" t="s">
-        <v>26</v>
-      </c>
-      <c r="E46" t="s">
-        <v>30</v>
-      </c>
-      <c r="F46">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" t="s">
-        <v>6</v>
-      </c>
-      <c r="B47" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="D58">
+        <v>0.8</v>
+      </c>
+      <c r="E58" t="s">
+        <v>32</v>
+      </c>
+      <c r="F58">
+        <v>0.7538095238095239</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59">
+        <v>6</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" t="s">
         <v>22</v>
       </c>
-      <c r="D47" t="s">
-        <v>27</v>
-      </c>
-      <c r="E47" t="s">
-        <v>28</v>
-      </c>
-      <c r="F47">
-        <v>0.8961285909712722</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" t="s">
-        <v>6</v>
-      </c>
-      <c r="B48" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="D59">
+        <v>0.2</v>
+      </c>
+      <c r="E59" t="s">
+        <v>30</v>
+      </c>
+      <c r="F59">
+        <v>0.9568946648426813</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60">
+        <v>6</v>
+      </c>
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" t="s">
         <v>22</v>
       </c>
-      <c r="D48" t="s">
-        <v>27</v>
-      </c>
-      <c r="E48" t="s">
-        <v>29</v>
-      </c>
-      <c r="F48">
+      <c r="D60">
+        <v>0.2</v>
+      </c>
+      <c r="E60" t="s">
+        <v>31</v>
+      </c>
+      <c r="F60">
+        <v>0.8766666666666666</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61">
+        <v>6</v>
+      </c>
+      <c r="B61" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" t="s">
+        <v>22</v>
+      </c>
+      <c r="D61">
+        <v>0.2</v>
+      </c>
+      <c r="E61" t="s">
+        <v>32</v>
+      </c>
+      <c r="F61">
+        <v>0.6523015873015873</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" t="s">
+        <v>23</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62" t="s">
+        <v>30</v>
+      </c>
+      <c r="F62">
+        <v>0.9300547195622435</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" t="s">
+        <v>23</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63" t="s">
+        <v>31</v>
+      </c>
+      <c r="F63">
         <v>0.02</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
-      <c r="A49" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" t="s">
-        <v>22</v>
-      </c>
-      <c r="D49" t="s">
-        <v>27</v>
-      </c>
-      <c r="E49" t="s">
-        <v>30</v>
-      </c>
-      <c r="F49">
-        <v>0.006666666666666668</v>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
+        <v>6</v>
+      </c>
+      <c r="B64" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" t="s">
+        <v>23</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64" t="s">
+        <v>32</v>
+      </c>
+      <c r="F64">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" t="s">
+        <v>24</v>
+      </c>
+      <c r="D65">
+        <v>0.1</v>
+      </c>
+      <c r="E65" t="s">
+        <v>30</v>
+      </c>
+      <c r="F65">
+        <v>0.5128454172366621</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" t="s">
+        <v>24</v>
+      </c>
+      <c r="D66">
+        <v>0.1</v>
+      </c>
+      <c r="E66" t="s">
+        <v>31</v>
+      </c>
+      <c r="F66">
+        <v>0.5033333333333333</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" t="s">
+        <v>24</v>
+      </c>
+      <c r="D67">
+        <v>0.1</v>
+      </c>
+      <c r="E67" t="s">
+        <v>32</v>
+      </c>
+      <c r="F67">
+        <v>0.06747642465944456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Branch and Bound normalizado
</commit_message>
<xml_diff>
--- a/model_results/all_models_results.xlsx
+++ b/model_results/all_models_results.xlsx
@@ -1,20 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Mestrado\projeto_SIN5007_rec_padroes\model_results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D634FDE-2640-4710-86B4-1E882293BA68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$73</definedName>
+  </definedNames>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="32">
   <si>
     <t>Atividade</t>
   </si>
@@ -34,7 +43,7 @@
     <t>Valor</t>
   </si>
   <si>
-    <t>6</t>
+    <t>7</t>
   </si>
   <si>
     <t>SVC</t>
@@ -61,12 +70,6 @@
     <t>PCA Balanceado</t>
   </si>
   <si>
-    <t>Branch and Bound - Sem Normalização - Desbalanceado</t>
-  </si>
-  <si>
-    <t>Branch and Bound - Sem Normalização - Balanceado</t>
-  </si>
-  <si>
     <t>Branch and Bound Desbalanceado - Nao Normalizado</t>
   </si>
   <si>
@@ -104,6 +107,9 @@
   </si>
   <si>
     <t>('sigmoid', 1, '0.0201')</t>
+  </si>
+  <si>
+    <t>('rbf', 1000, '0.9401')</t>
   </si>
   <si>
     <t>Accuracy</t>
@@ -118,8 +124,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,11 +188,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -228,7 +242,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -260,9 +274,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -294,6 +326,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -469,14 +519,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,7 +556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>7</v>
       </c>
@@ -507,16 +567,16 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2">
-        <v>0.9603830369357045</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0.96038303693570448</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>7</v>
       </c>
@@ -527,16 +587,16 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3">
         <v>0.86</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7</v>
       </c>
@@ -547,16 +607,16 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4">
         <v>0.677579365079365</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7</v>
       </c>
@@ -567,16 +627,16 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5">
-        <v>0.9627086183310534</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>0.96270861833105337</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7</v>
       </c>
@@ -587,16 +647,16 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6">
-        <v>0.8766666666666666</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>0.87666666666666659</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -607,16 +667,16 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7">
-        <v>0.6900793650793651</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>0.69007936507936507</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -627,16 +687,16 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8">
-        <v>0.9627086183310534</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>0.96270861833105337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -647,16 +707,16 @@
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9">
-        <v>0.8766666666666666</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>0.87666666666666659</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -667,16 +727,16 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10">
-        <v>0.6900793650793651</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>0.69007936507936507</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -687,16 +747,16 @@
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11">
-        <v>0.9591928864569083</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>0.95919288645690826</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7</v>
       </c>
@@ -707,16 +767,16 @@
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F12">
-        <v>0.9100000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>0.91000000000000014</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -727,16 +787,16 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13">
-        <v>0.6730158730158731</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>0.67301587301587307</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
@@ -747,16 +807,16 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F14">
-        <v>0.9638987688098494</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>0.96389876880984937</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
@@ -767,16 +827,16 @@
         <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F15">
         <v>0.6399999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>7</v>
       </c>
@@ -787,16 +847,16 @@
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16">
-        <v>0.7995238095238095</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>0.79952380952380953</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>7</v>
       </c>
@@ -807,16 +867,16 @@
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F17">
         <v>0.9580574555403556</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7</v>
       </c>
@@ -827,16 +887,16 @@
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F18">
-        <v>0.7166666666666666</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>0.71666666666666656</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>7</v>
       </c>
@@ -847,16 +907,16 @@
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F19">
-        <v>0.7138095238095238</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>0.71380952380952378</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>7</v>
       </c>
@@ -867,16 +927,16 @@
         <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F20">
-        <v>0.9382352941176469</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>0.93823529411764695</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>7</v>
       </c>
@@ -887,16 +947,16 @@
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F21">
-        <v>0.08333333333333333</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>7</v>
       </c>
@@ -907,16 +967,16 @@
         <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F22">
         <v>0.35</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>7</v>
       </c>
@@ -927,16 +987,16 @@
         <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F23">
-        <v>0.8961285909712722</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>0.89612859097127218</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>7</v>
       </c>
@@ -947,16 +1007,16 @@
         <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F24">
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>7</v>
       </c>
@@ -967,16 +1027,16 @@
         <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F25">
-        <v>0.006666666666666668</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>6.666666666666668E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6</v>
       </c>
@@ -984,19 +1044,19 @@
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D26">
         <v>0.6</v>
       </c>
       <c r="E26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F26">
-        <v>0.9312448700410396</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>0.93124487004103962</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>6</v>
       </c>
@@ -1004,19 +1064,19 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D27">
         <v>0.6</v>
       </c>
       <c r="E27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6</v>
       </c>
@@ -1024,19 +1084,19 @@
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D28">
         <v>0.6</v>
       </c>
       <c r="E28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F28">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6</v>
       </c>
@@ -1044,19 +1104,19 @@
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D29">
         <v>0.3</v>
       </c>
       <c r="E29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F29">
-        <v>0.6901094391244869</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>0.69010943912448686</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6</v>
       </c>
@@ -1064,19 +1124,19 @@
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D30">
         <v>0.3</v>
       </c>
       <c r="E30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F30">
         <v>0.2166666666666667</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>6</v>
       </c>
@@ -1084,19 +1144,19 @@
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D31">
         <v>0.3</v>
       </c>
       <c r="E31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F31">
-        <v>0.04927119294207902</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>4.9271192942079017E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>6</v>
       </c>
@@ -1110,13 +1170,13 @@
         <v>0.9</v>
       </c>
       <c r="E32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F32">
-        <v>0.9335567715458277</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>0.93355677154582772</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>6</v>
       </c>
@@ -1130,13 +1190,13 @@
         <v>0.9</v>
       </c>
       <c r="E33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F33">
         <v>0.11</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>6</v>
       </c>
@@ -1150,13 +1210,13 @@
         <v>0.9</v>
       </c>
       <c r="E34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F34">
-        <v>0.2166666666666666</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>0.21666666666666659</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>6</v>
       </c>
@@ -1170,13 +1230,13 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F35">
-        <v>0.9428590971272228</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>0.94285909712722282</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>6</v>
       </c>
@@ -1190,13 +1250,13 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F36">
         <v>0.64</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>6</v>
       </c>
@@ -1210,13 +1270,13 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F37">
-        <v>0.5904761904761904</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>0.59047619047619038</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>6</v>
       </c>
@@ -1224,19 +1284,19 @@
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D38">
         <v>0.4</v>
       </c>
       <c r="E38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F38">
-        <v>0.9627222982216141</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>0.96272229822161415</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>6</v>
       </c>
@@ -1244,19 +1304,19 @@
         <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D39">
         <v>0.4</v>
       </c>
       <c r="E39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F39">
-        <v>0.6966666666666667</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>0.69666666666666666</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>6</v>
       </c>
@@ -1264,19 +1324,19 @@
         <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D40">
         <v>0.4</v>
       </c>
       <c r="E40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F40">
-        <v>0.7538095238095239</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>0.75380952380952393</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>6</v>
       </c>
@@ -1284,19 +1344,19 @@
         <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D41">
         <v>0.1</v>
       </c>
       <c r="E41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F41">
-        <v>0.9568946648426813</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>0.95689466484268126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>6</v>
       </c>
@@ -1304,19 +1364,19 @@
         <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D42">
         <v>0.1</v>
       </c>
       <c r="E42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F42">
-        <v>0.8766666666666666</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>0.87666666666666659</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>6</v>
       </c>
@@ -1324,19 +1384,19 @@
         <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D43">
         <v>0.1</v>
       </c>
       <c r="E43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F43">
-        <v>0.6523015873015873</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>0.65230158730158727</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>6</v>
       </c>
@@ -1350,13 +1410,13 @@
         <v>0.6</v>
       </c>
       <c r="E44" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F44">
-        <v>0.9556771545827634</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>0.95567715458276337</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>6</v>
       </c>
@@ -1370,13 +1430,13 @@
         <v>0.6</v>
       </c>
       <c r="E45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F45">
-        <v>0.7166666666666666</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>0.71666666666666656</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>6</v>
       </c>
@@ -1390,13 +1450,13 @@
         <v>0.6</v>
       </c>
       <c r="E46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F46">
-        <v>0.6753968253968254</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>0.67539682539682544</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>6</v>
       </c>
@@ -1410,13 +1470,13 @@
         <v>0.8</v>
       </c>
       <c r="E47" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F47">
-        <v>0.9393296853625172</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>0.93932968536251715</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>6</v>
       </c>
@@ -1430,13 +1490,13 @@
         <v>0.8</v>
       </c>
       <c r="E48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F48">
-        <v>0.8766666666666666</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+        <v>0.87666666666666659</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>6</v>
       </c>
@@ -1450,13 +1510,13 @@
         <v>0.8</v>
       </c>
       <c r="E49" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F49">
-        <v>0.547142857142857</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+        <v>0.54714285714285704</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>6</v>
       </c>
@@ -1470,13 +1530,13 @@
         <v>0.9</v>
       </c>
       <c r="E50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F50">
-        <v>0.9475376196990425</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
+        <v>0.94753761969904249</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>6</v>
       </c>
@@ -1490,13 +1550,13 @@
         <v>0.9</v>
       </c>
       <c r="E51" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F51">
-        <v>0.7166666666666666</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+        <v>0.71666666666666656</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>6</v>
       </c>
@@ -1510,13 +1570,13 @@
         <v>0.9</v>
       </c>
       <c r="E52" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F52">
-        <v>0.6044444444444445</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+        <v>0.60444444444444445</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>6</v>
       </c>
@@ -1530,13 +1590,13 @@
         <v>0.2</v>
       </c>
       <c r="E53" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F53">
-        <v>0.9358413132694938</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+        <v>0.93584131326949382</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>6</v>
       </c>
@@ -1550,13 +1610,13 @@
         <v>0.2</v>
       </c>
       <c r="E54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F54">
-        <v>0.8766666666666666</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
+        <v>0.87666666666666659</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>6</v>
       </c>
@@ -1570,13 +1630,13 @@
         <v>0.2</v>
       </c>
       <c r="E55" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F55">
-        <v>0.5276984126984127</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
+        <v>0.52769841269841267</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>6</v>
       </c>
@@ -1584,19 +1644,19 @@
         <v>8</v>
       </c>
       <c r="C56" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D56">
         <v>0.8</v>
       </c>
       <c r="E56" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F56">
-        <v>0.9627222982216141</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
+        <v>0.96272229822161415</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>6</v>
       </c>
@@ -1604,19 +1664,19 @@
         <v>8</v>
       </c>
       <c r="C57" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D57">
         <v>0.8</v>
       </c>
       <c r="E57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F57">
-        <v>0.6966666666666667</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+        <v>0.69666666666666666</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>6</v>
       </c>
@@ -1624,19 +1684,19 @@
         <v>8</v>
       </c>
       <c r="C58" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D58">
         <v>0.8</v>
       </c>
       <c r="E58" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F58">
-        <v>0.7538095238095239</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
+        <v>0.75380952380952393</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>6</v>
       </c>
@@ -1644,19 +1704,19 @@
         <v>8</v>
       </c>
       <c r="C59" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D59">
         <v>0.2</v>
       </c>
       <c r="E59" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F59">
-        <v>0.9568946648426813</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
+        <v>0.95689466484268126</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>6</v>
       </c>
@@ -1664,19 +1724,19 @@
         <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D60">
         <v>0.2</v>
       </c>
       <c r="E60" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F60">
-        <v>0.8766666666666666</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
+        <v>0.87666666666666659</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>6</v>
       </c>
@@ -1684,139 +1744,260 @@
         <v>8</v>
       </c>
       <c r="C61" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D61">
         <v>0.2</v>
       </c>
       <c r="E61" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F61">
-        <v>0.6523015873015873</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62" t="s">
+        <v>0.65230158730158727</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62">
         <v>6</v>
       </c>
       <c r="B62" t="s">
         <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D62">
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F62">
         <v>0.9300547195622435</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
-      <c r="A63" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63">
         <v>6</v>
       </c>
       <c r="B63" t="s">
         <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D63">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F63">
         <v>0.02</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
-      <c r="A64" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64">
         <v>6</v>
       </c>
       <c r="B64" t="s">
         <v>8</v>
       </c>
       <c r="C64" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D64">
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F64">
         <v>0.1</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
-      <c r="A65" t="s">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65">
         <v>6</v>
       </c>
       <c r="B65" t="s">
         <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D65">
         <v>0.1</v>
       </c>
       <c r="E65" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F65">
         <v>0.5128454172366621</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
-      <c r="A66" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66">
         <v>6</v>
       </c>
       <c r="B66" t="s">
         <v>8</v>
       </c>
       <c r="C66" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D66">
         <v>0.1</v>
       </c>
       <c r="E66" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F66">
         <v>0.5033333333333333</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
-      <c r="A67" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67">
         <v>6</v>
       </c>
       <c r="B67" t="s">
         <v>8</v>
       </c>
       <c r="C67" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D67">
         <v>0.1</v>
       </c>
       <c r="E67" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F67">
-        <v>0.06747642465944456</v>
+        <v>6.7476424659444562E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" t="s">
+        <v>21</v>
+      </c>
+      <c r="D68" t="s">
+        <v>23</v>
+      </c>
+      <c r="E68" t="s">
+        <v>29</v>
+      </c>
+      <c r="F68">
+        <v>0.93590971272229828</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" t="s">
+        <v>21</v>
+      </c>
+      <c r="D69" t="s">
+        <v>23</v>
+      </c>
+      <c r="E69" t="s">
+        <v>30</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" t="s">
+        <v>21</v>
+      </c>
+      <c r="D70" t="s">
+        <v>23</v>
+      </c>
+      <c r="E70" t="s">
+        <v>31</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" t="s">
+        <v>22</v>
+      </c>
+      <c r="D71" t="s">
+        <v>28</v>
+      </c>
+      <c r="E71" t="s">
+        <v>29</v>
+      </c>
+      <c r="F71">
+        <v>0.82288645690834472</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" t="s">
+        <v>22</v>
+      </c>
+      <c r="D72" t="s">
+        <v>28</v>
+      </c>
+      <c r="E72" t="s">
+        <v>30</v>
+      </c>
+      <c r="F72">
+        <v>0.15333333333333329</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" t="s">
+        <v>22</v>
+      </c>
+      <c r="D73" t="s">
+        <v>28</v>
+      </c>
+      <c r="E73" t="s">
+        <v>31</v>
+      </c>
+      <c r="F73">
+        <v>9.0642135642135649E-2</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F73" xr:uid="{403F961F-3202-4180-B00F-57FB763DEF50}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MLP duas camadas ocultas
</commit_message>
<xml_diff>
--- a/model_results/all_models_results.xlsx
+++ b/model_results/all_models_results.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LHS\Documents\GitHub\projeto_SIN5007_rec_padroes\model_results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155AF734-F489-4FA9-82F1-0D12B7DBF3A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="139">
   <si>
     <t>Algoritmo</t>
   </si>
@@ -118,40 +124,40 @@
     <t>('rbf', 1, '0.10010000000000001')</t>
   </si>
   <si>
-    <t>(6, 0.001, 'logistic')</t>
-  </si>
-  <si>
-    <t>(6, 0.003, 'relu')</t>
-  </si>
-  <si>
-    <t>(7, 0.004, 'relu')</t>
-  </si>
-  <si>
-    <t>(9, 0.001, 'relu')</t>
-  </si>
-  <si>
-    <t>(8, 0.003, 'logistic')</t>
-  </si>
-  <si>
-    <t>(9, 0.009000000000000001, 'tanh')</t>
-  </si>
-  <si>
-    <t>(9, 0.003, 'logistic')</t>
-  </si>
-  <si>
-    <t>(7, 0.008, 'relu')</t>
-  </si>
-  <si>
-    <t>(9, 0.002, 'relu')</t>
-  </si>
-  <si>
-    <t>(6, 0.009000000000000001, 'logistic')</t>
-  </si>
-  <si>
-    <t>(8, 0.003, 'tanh')</t>
-  </si>
-  <si>
-    <t>(9, 0.006999999999999999, 'tanh')</t>
+    <t>((5, 7), 0.01, 'relu', 0.9, 300, False)</t>
+  </si>
+  <si>
+    <t>((15, 10), 0.001, 'relu', 0.9, 300, False)</t>
+  </si>
+  <si>
+    <t>((5,), 0.001, 'logistic', 0.3, 300, False)</t>
+  </si>
+  <si>
+    <t>((10,), 0.01, 'logistic', 0.9, 300, False)</t>
+  </si>
+  <si>
+    <t>((5, 5), 0.1, 'relu', 0.3, 300, True)</t>
+  </si>
+  <si>
+    <t>((10, 7), 0.01, 'relu', 0.6, 300, False)</t>
+  </si>
+  <si>
+    <t>((7,), 0.001, 'relu', 0.9, 300, False)</t>
+  </si>
+  <si>
+    <t>((5, 20), 0.1, 'logistic', 0.6, 300, False)</t>
+  </si>
+  <si>
+    <t>((10, 15), 0.1, 'relu', 0.9, 300, False)</t>
+  </si>
+  <si>
+    <t>((5,), 0.01, 'relu', 0.9, 300, True)</t>
+  </si>
+  <si>
+    <t>((5, 7), 0.1, 'relu', 0.3, 300, False)</t>
+  </si>
+  <si>
+    <t>((7,), 0.001, 'tanh', 0.6, 300, False)</t>
   </si>
   <si>
     <t>Accuracy</t>
@@ -355,107 +361,89 @@
     <t>[0.7366666666666666, 0.5743750030070749, 0.8989583303262583]</t>
   </si>
   <si>
-    <t>[0.672, 0.523, 0.821]</t>
-  </si>
-  <si>
-    <t>[0.333, 0.068, 0.598]</t>
-  </si>
-  <si>
-    <t>[0.063, 0.009, 0.117]</t>
-  </si>
-  <si>
-    <t>[0.964, 0.943, 0.985]</t>
-  </si>
-  <si>
-    <t>[0.723, 0.492, 0.954]</t>
-  </si>
-  <si>
-    <t>[0.685, 0.469, 0.901]</t>
-  </si>
-  <si>
-    <t>[0.958, 0.940, 0.976]</t>
-  </si>
-  <si>
-    <t>[0.655, 0.538, 0.771]</t>
-  </si>
-  <si>
-    <t>[0.637, 0.506, 0.767]</t>
-  </si>
-  <si>
-    <t>[0.766, 0.606, 0.927]</t>
-  </si>
-  <si>
-    <t>[0.950, 0.930, 0.970]</t>
-  </si>
-  <si>
-    <t>[0.727, 0.585, 0.868]</t>
-  </si>
-  <si>
-    <t>[0.608, 0.466, 0.750]</t>
-  </si>
-  <si>
-    <t>[0.962, 0.944, 0.979]</t>
-  </si>
-  <si>
-    <t>[0.577, 0.394, 0.760]</t>
-  </si>
-  <si>
-    <t>[0.710, 0.475, 0.944]</t>
-  </si>
-  <si>
-    <t>[0.843, 0.724, 0.963]</t>
-  </si>
-  <si>
-    <t>[0.962, 0.947, 0.976]</t>
-  </si>
-  <si>
-    <t>[0.577, 0.420, 0.733]</t>
-  </si>
-  <si>
-    <t>[0.753, 0.596, 0.910]</t>
-  </si>
-  <si>
-    <t>[0.953, 0.933, 0.973]</t>
-  </si>
-  <si>
-    <t>[0.800, 0.676, 0.924]</t>
-  </si>
-  <si>
-    <t>[0.636, 0.488, 0.785]</t>
-  </si>
-  <si>
-    <t>[0.959, 0.943, 0.975]</t>
-  </si>
-  <si>
-    <t>[0.657, 0.521, 0.792]</t>
-  </si>
-  <si>
-    <t>[0.693, 0.557, 0.830]</t>
-  </si>
-  <si>
-    <t>[0.952, 0.933, 0.971]</t>
-  </si>
-  <si>
-    <t>[0.767, 0.651, 0.882]</t>
-  </si>
-  <si>
-    <t>[0.627, 0.501, 0.753]</t>
-  </si>
-  <si>
-    <t>[0.683, 0.631, 0.735]</t>
-  </si>
-  <si>
-    <t>[0.247, 0.094, 0.399]</t>
-  </si>
-  <si>
-    <t>[0.060, 0.019, 0.100]</t>
+    <t>[0.956, 0.939, 0.972]</t>
+  </si>
+  <si>
+    <t>[0.597, 0.398, 0.796]</t>
+  </si>
+  <si>
+    <t>[0.693, 0.539, 0.846]</t>
+  </si>
+  <si>
+    <t>[0.958, 0.939, 0.977]</t>
+  </si>
+  <si>
+    <t>[0.840, 0.750, 0.930]</t>
+  </si>
+  <si>
+    <t>[0.667, 0.534, 0.801]</t>
+  </si>
+  <si>
+    <t>[0.965, 0.948, 0.982]</t>
+  </si>
+  <si>
+    <t>[0.677, 0.556, 0.797]</t>
+  </si>
+  <si>
+    <t>[0.781, 0.626, 0.936]</t>
+  </si>
+  <si>
+    <t>[0.956, 0.938, 0.973]</t>
+  </si>
+  <si>
+    <t>[0.877, 0.776, 0.977]</t>
+  </si>
+  <si>
+    <t>[0.629, 0.514, 0.743]</t>
+  </si>
+  <si>
+    <t>[0.952, 0.942, 0.962]</t>
+  </si>
+  <si>
+    <t>[0.327, 0.137, 0.516]</t>
+  </si>
+  <si>
+    <t>[0.557, 0.255, 0.858]</t>
+  </si>
+  <si>
+    <t>[0.966, 0.951, 0.981]</t>
+  </si>
+  <si>
+    <t>[0.627, 0.433, 0.820]</t>
+  </si>
+  <si>
+    <t>[0.738, 0.513, 0.963]</t>
+  </si>
+  <si>
+    <t>[0.670, 0.505, 0.835]</t>
+  </si>
+  <si>
+    <t>[0.672, 0.533, 0.810]</t>
+  </si>
+  <si>
+    <t>[0.937, 0.931, 0.943]</t>
+  </si>
+  <si>
+    <t>[0.040, -0.020, 0.100]</t>
+  </si>
+  <si>
+    <t>[0.150, -0.091, 0.391]</t>
+  </si>
+  <si>
+    <t>[0.966, 0.948, 0.984]</t>
+  </si>
+  <si>
+    <t>[0.770, 0.582, 0.958]</t>
+  </si>
+  <si>
+    <t>[0.748, 0.600, 0.896]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -518,6 +506,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -564,7 +560,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -596,9 +592,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -630,6 +644,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -805,14 +837,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="A127" sqref="A86:XFD127"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="47.5703125" customWidth="1"/>
+    <col min="4" max="4" width="64.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -835,7 +873,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -852,13 +890,13 @@
         <v>46</v>
       </c>
       <c r="F2">
-        <v>0.8961285909712722</v>
+        <v>0.89612859097127218</v>
       </c>
       <c r="G2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -881,7 +919,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -898,13 +936,13 @@
         <v>48</v>
       </c>
       <c r="F4">
-        <v>0.006666666666666668</v>
+        <v>6.666666666666668E-3</v>
       </c>
       <c r="G4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -921,13 +959,13 @@
         <v>46</v>
       </c>
       <c r="F5">
-        <v>0.6901094391244869</v>
+        <v>0.69010943912448686</v>
       </c>
       <c r="G5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -950,7 +988,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -967,13 +1005,13 @@
         <v>48</v>
       </c>
       <c r="F7">
-        <v>0.04927119294207902</v>
+        <v>4.9271192942079017E-2</v>
       </c>
       <c r="G7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -990,13 +1028,13 @@
         <v>46</v>
       </c>
       <c r="F8">
-        <v>0.8228864569083447</v>
+        <v>0.82288645690834472</v>
       </c>
       <c r="G8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1013,13 +1051,13 @@
         <v>47</v>
       </c>
       <c r="F9">
-        <v>0.1533333333333333</v>
+        <v>0.15333333333333329</v>
       </c>
       <c r="G9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1036,13 +1074,13 @@
         <v>48</v>
       </c>
       <c r="F10">
-        <v>0.09064213564213565</v>
+        <v>9.0642135642135649E-2</v>
       </c>
       <c r="G10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1065,7 +1103,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1088,7 +1126,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1105,13 +1143,13 @@
         <v>48</v>
       </c>
       <c r="F13">
-        <v>0.06747642465944456</v>
+        <v>6.7476424659444562E-2</v>
       </c>
       <c r="G13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1128,13 +1166,13 @@
         <v>46</v>
       </c>
       <c r="F14">
-        <v>0.9382352941176469</v>
+        <v>0.93823529411764695</v>
       </c>
       <c r="G14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1151,13 +1189,13 @@
         <v>47</v>
       </c>
       <c r="F15">
-        <v>0.08333333333333333</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="G15" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1180,7 +1218,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1197,13 +1235,13 @@
         <v>46</v>
       </c>
       <c r="F17">
-        <v>0.9312448700410396</v>
+        <v>0.93124487004103962</v>
       </c>
       <c r="G17" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1226,7 +1264,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1249,7 +1287,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1266,13 +1304,13 @@
         <v>46</v>
       </c>
       <c r="F20">
-        <v>0.9359097127222983</v>
+        <v>0.93590971272229828</v>
       </c>
       <c r="G20" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1295,7 +1333,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1318,7 +1356,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1341,7 +1379,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1364,7 +1402,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1387,7 +1425,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1404,13 +1442,13 @@
         <v>46</v>
       </c>
       <c r="F26">
-        <v>0.9627086183310534</v>
+        <v>0.96270861833105337</v>
       </c>
       <c r="G26" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1427,13 +1465,13 @@
         <v>47</v>
       </c>
       <c r="F27">
-        <v>0.8766666666666666</v>
+        <v>0.87666666666666659</v>
       </c>
       <c r="G27" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1450,13 +1488,13 @@
         <v>48</v>
       </c>
       <c r="F28">
-        <v>0.6900793650793651</v>
+        <v>0.69007936507936507</v>
       </c>
       <c r="G28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1473,13 +1511,13 @@
         <v>46</v>
       </c>
       <c r="F29">
-        <v>0.9393296853625172</v>
+        <v>0.93932968536251715</v>
       </c>
       <c r="G29" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1496,13 +1534,13 @@
         <v>47</v>
       </c>
       <c r="F30">
-        <v>0.8766666666666666</v>
+        <v>0.87666666666666659</v>
       </c>
       <c r="G30" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1519,13 +1557,13 @@
         <v>48</v>
       </c>
       <c r="F31">
-        <v>0.547142857142857</v>
+        <v>0.54714285714285704</v>
       </c>
       <c r="G31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1542,13 +1580,13 @@
         <v>46</v>
       </c>
       <c r="F32">
-        <v>0.9591928864569083</v>
+        <v>0.95919288645690826</v>
       </c>
       <c r="G32" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -1565,13 +1603,13 @@
         <v>47</v>
       </c>
       <c r="F33">
-        <v>0.9100000000000001</v>
+        <v>0.91000000000000014</v>
       </c>
       <c r="G33" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -1588,13 +1626,13 @@
         <v>48</v>
       </c>
       <c r="F34">
-        <v>0.6730158730158731</v>
+        <v>0.67301587301587307</v>
       </c>
       <c r="G34" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -1611,13 +1649,13 @@
         <v>46</v>
       </c>
       <c r="F35">
-        <v>0.9358413132694938</v>
+        <v>0.93584131326949382</v>
       </c>
       <c r="G35" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -1634,13 +1672,13 @@
         <v>47</v>
       </c>
       <c r="F36">
-        <v>0.8766666666666666</v>
+        <v>0.87666666666666659</v>
       </c>
       <c r="G36" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -1657,13 +1695,13 @@
         <v>48</v>
       </c>
       <c r="F37">
-        <v>0.5276984126984127</v>
+        <v>0.52769841269841267</v>
       </c>
       <c r="G37" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -1680,13 +1718,13 @@
         <v>46</v>
       </c>
       <c r="F38">
-        <v>0.9603830369357045</v>
+        <v>0.96038303693570448</v>
       </c>
       <c r="G38" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1709,7 +1747,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -1732,7 +1770,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -1749,13 +1787,13 @@
         <v>46</v>
       </c>
       <c r="F41">
-        <v>0.9556771545827634</v>
+        <v>0.95567715458276337</v>
       </c>
       <c r="G41" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -1772,13 +1810,13 @@
         <v>47</v>
       </c>
       <c r="F42">
-        <v>0.7166666666666666</v>
+        <v>0.71666666666666656</v>
       </c>
       <c r="G42" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -1795,13 +1833,13 @@
         <v>48</v>
       </c>
       <c r="F43">
-        <v>0.6753968253968254</v>
+        <v>0.67539682539682544</v>
       </c>
       <c r="G43" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -1818,13 +1856,13 @@
         <v>46</v>
       </c>
       <c r="F44">
-        <v>0.9627086183310534</v>
+        <v>0.96270861833105337</v>
       </c>
       <c r="G44" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -1841,13 +1879,13 @@
         <v>47</v>
       </c>
       <c r="F45">
-        <v>0.8766666666666666</v>
+        <v>0.87666666666666659</v>
       </c>
       <c r="G45" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -1864,13 +1902,13 @@
         <v>48</v>
       </c>
       <c r="F46">
-        <v>0.6900793650793651</v>
+        <v>0.69007936507936507</v>
       </c>
       <c r="G46" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -1887,13 +1925,13 @@
         <v>46</v>
       </c>
       <c r="F47">
-        <v>0.9475376196990425</v>
+        <v>0.94753761969904249</v>
       </c>
       <c r="G47" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -1910,13 +1948,13 @@
         <v>47</v>
       </c>
       <c r="F48">
-        <v>0.7166666666666666</v>
+        <v>0.71666666666666656</v>
       </c>
       <c r="G48" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -1933,13 +1971,13 @@
         <v>48</v>
       </c>
       <c r="F49">
-        <v>0.6044444444444445</v>
+        <v>0.60444444444444445</v>
       </c>
       <c r="G49" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -1962,7 +2000,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -1979,13 +2017,13 @@
         <v>47</v>
       </c>
       <c r="F51">
-        <v>0.7166666666666666</v>
+        <v>0.71666666666666656</v>
       </c>
       <c r="G51" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -2002,13 +2040,13 @@
         <v>48</v>
       </c>
       <c r="F52">
-        <v>0.7138095238095238</v>
+        <v>0.71380952380952378</v>
       </c>
       <c r="G52" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -2025,13 +2063,13 @@
         <v>46</v>
       </c>
       <c r="F53">
-        <v>0.9416963064295485</v>
+        <v>0.94169630642954849</v>
       </c>
       <c r="G53" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -2054,7 +2092,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>8</v>
       </c>
@@ -2071,13 +2109,13 @@
         <v>48</v>
       </c>
       <c r="F55">
-        <v>0.5704761904761905</v>
+        <v>0.57047619047619047</v>
       </c>
       <c r="G55" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -2094,13 +2132,13 @@
         <v>46</v>
       </c>
       <c r="F56">
-        <v>0.9638987688098494</v>
+        <v>0.96389876880984937</v>
       </c>
       <c r="G56" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -2123,7 +2161,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -2140,13 +2178,13 @@
         <v>48</v>
       </c>
       <c r="F58">
-        <v>0.7995238095238095</v>
+        <v>0.79952380952380953</v>
       </c>
       <c r="G58" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -2163,13 +2201,13 @@
         <v>46</v>
       </c>
       <c r="F59">
-        <v>0.9335567715458277</v>
+        <v>0.93355677154582772</v>
       </c>
       <c r="G59" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -2192,7 +2230,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -2209,13 +2247,13 @@
         <v>48</v>
       </c>
       <c r="F61">
-        <v>0.2166666666666666</v>
+        <v>0.21666666666666659</v>
       </c>
       <c r="G61" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>7</v>
       </c>
@@ -2232,13 +2270,13 @@
         <v>46</v>
       </c>
       <c r="F62">
-        <v>0.9627086183310534</v>
+        <v>0.96270861833105337</v>
       </c>
       <c r="G62" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>7</v>
       </c>
@@ -2255,13 +2293,13 @@
         <v>47</v>
       </c>
       <c r="F63">
-        <v>0.8766666666666666</v>
+        <v>0.87666666666666659</v>
       </c>
       <c r="G63" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>7</v>
       </c>
@@ -2278,13 +2316,13 @@
         <v>48</v>
       </c>
       <c r="F64">
-        <v>0.6900793650793651</v>
+        <v>0.69007936507936507</v>
       </c>
       <c r="G64" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>8</v>
       </c>
@@ -2301,13 +2339,13 @@
         <v>46</v>
       </c>
       <c r="F65">
-        <v>0.9568946648426813</v>
+        <v>0.95689466484268126</v>
       </c>
       <c r="G65" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -2324,13 +2362,13 @@
         <v>47</v>
       </c>
       <c r="F66">
-        <v>0.8766666666666666</v>
+        <v>0.87666666666666659</v>
       </c>
       <c r="G66" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>8</v>
       </c>
@@ -2347,13 +2385,13 @@
         <v>48</v>
       </c>
       <c r="F67">
-        <v>0.6523015873015873</v>
+        <v>0.65230158730158727</v>
       </c>
       <c r="G67" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -2376,7 +2414,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>7</v>
       </c>
@@ -2393,13 +2431,13 @@
         <v>47</v>
       </c>
       <c r="F69">
-        <v>0.8766666666666666</v>
+        <v>0.87666666666666659</v>
       </c>
       <c r="G69" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>7</v>
       </c>
@@ -2416,13 +2454,13 @@
         <v>48</v>
       </c>
       <c r="F70">
-        <v>0.6972222222222222</v>
+        <v>0.69722222222222219</v>
       </c>
       <c r="G70" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>8</v>
       </c>
@@ -2439,13 +2477,13 @@
         <v>46</v>
       </c>
       <c r="F71">
-        <v>0.9568946648426813</v>
+        <v>0.95689466484268126</v>
       </c>
       <c r="G71" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>8</v>
       </c>
@@ -2462,13 +2500,13 @@
         <v>47</v>
       </c>
       <c r="F72">
-        <v>0.8766666666666666</v>
+        <v>0.87666666666666659</v>
       </c>
       <c r="G72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>8</v>
       </c>
@@ -2485,13 +2523,13 @@
         <v>48</v>
       </c>
       <c r="F73">
-        <v>0.6523015873015873</v>
+        <v>0.65230158730158727</v>
       </c>
       <c r="G73" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>7</v>
       </c>
@@ -2508,13 +2546,13 @@
         <v>46</v>
       </c>
       <c r="F74">
-        <v>0.9615458276333788</v>
+        <v>0.96154582763337881</v>
       </c>
       <c r="G74" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>7</v>
       </c>
@@ -2531,13 +2569,13 @@
         <v>47</v>
       </c>
       <c r="F75">
-        <v>0.8766666666666666</v>
+        <v>0.87666666666666659</v>
       </c>
       <c r="G75" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>7</v>
       </c>
@@ -2554,13 +2592,13 @@
         <v>48</v>
       </c>
       <c r="F76">
-        <v>0.6831349206349205</v>
+        <v>0.68313492063492054</v>
       </c>
       <c r="G76" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>8</v>
       </c>
@@ -2577,13 +2615,13 @@
         <v>46</v>
       </c>
       <c r="F77">
-        <v>0.9627222982216141</v>
+        <v>0.96272229822161415</v>
       </c>
       <c r="G77" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>8</v>
       </c>
@@ -2600,13 +2638,13 @@
         <v>47</v>
       </c>
       <c r="F78">
-        <v>0.6966666666666667</v>
+        <v>0.69666666666666666</v>
       </c>
       <c r="G78" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>8</v>
       </c>
@@ -2623,13 +2661,13 @@
         <v>48</v>
       </c>
       <c r="F79">
-        <v>0.7538095238095239</v>
+        <v>0.75380952380952393</v>
       </c>
       <c r="G79" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>7</v>
       </c>
@@ -2646,13 +2684,13 @@
         <v>46</v>
       </c>
       <c r="F80">
-        <v>0.961545827633379</v>
+        <v>0.96154582763337904</v>
       </c>
       <c r="G80" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>7</v>
       </c>
@@ -2669,13 +2707,13 @@
         <v>47</v>
       </c>
       <c r="F81">
-        <v>0.6599999999999999</v>
+        <v>0.65999999999999992</v>
       </c>
       <c r="G81" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>7</v>
       </c>
@@ -2692,13 +2730,13 @@
         <v>48</v>
       </c>
       <c r="F82">
-        <v>0.7366666666666666</v>
+        <v>0.73666666666666658</v>
       </c>
       <c r="G82" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>8</v>
       </c>
@@ -2715,13 +2753,13 @@
         <v>46</v>
       </c>
       <c r="F83">
-        <v>0.9627222982216141</v>
+        <v>0.96272229822161415</v>
       </c>
       <c r="G83" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>8</v>
       </c>
@@ -2738,13 +2776,13 @@
         <v>47</v>
       </c>
       <c r="F84">
-        <v>0.6966666666666667</v>
+        <v>0.69666666666666666</v>
       </c>
       <c r="G84" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>8</v>
       </c>
@@ -2761,13 +2799,13 @@
         <v>48</v>
       </c>
       <c r="F85">
-        <v>0.7538095238095239</v>
+        <v>0.75380952380952393</v>
       </c>
       <c r="G85" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>9</v>
       </c>
@@ -2775,7 +2813,7 @@
         <v>8</v>
       </c>
       <c r="C86" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D86" t="s">
         <v>34</v>
@@ -2784,13 +2822,13 @@
         <v>46</v>
       </c>
       <c r="F86">
-        <v>0.9359097127222983</v>
+        <v>0.95570451436388504</v>
       </c>
       <c r="G86" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>9</v>
       </c>
@@ -2798,7 +2836,7 @@
         <v>8</v>
       </c>
       <c r="C87" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D87" t="s">
         <v>34</v>
@@ -2807,13 +2845,13 @@
         <v>47</v>
       </c>
       <c r="F87">
-        <v>0</v>
+        <v>0.59666666666666668</v>
       </c>
       <c r="G87" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>9</v>
       </c>
@@ -2821,7 +2859,7 @@
         <v>8</v>
       </c>
       <c r="C88" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D88" t="s">
         <v>34</v>
@@ -2830,13 +2868,13 @@
         <v>48</v>
       </c>
       <c r="F88">
-        <v>0</v>
+        <v>0.69261904761904758</v>
       </c>
       <c r="G88" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>9</v>
       </c>
@@ -2844,7 +2882,7 @@
         <v>8</v>
       </c>
       <c r="C89" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D89" t="s">
         <v>35</v>
@@ -2853,13 +2891,13 @@
         <v>46</v>
       </c>
       <c r="F89">
-        <v>0.6724897400820793</v>
+        <v>0.95801641586867292</v>
       </c>
       <c r="G89" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>9</v>
       </c>
@@ -2867,7 +2905,7 @@
         <v>8</v>
       </c>
       <c r="C90" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D90" t="s">
         <v>35</v>
@@ -2876,13 +2914,13 @@
         <v>47</v>
       </c>
       <c r="F90">
-        <v>0.3333333333333334</v>
+        <v>0.84000000000000008</v>
       </c>
       <c r="G90" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>9</v>
       </c>
@@ -2890,7 +2928,7 @@
         <v>8</v>
       </c>
       <c r="C91" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D91" t="s">
         <v>35</v>
@@ -2899,13 +2937,13 @@
         <v>48</v>
       </c>
       <c r="F91">
-        <v>0.06324528810898969</v>
+        <v>0.66731601731601731</v>
       </c>
       <c r="G91" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>9</v>
       </c>
@@ -2913,7 +2951,7 @@
         <v>8</v>
       </c>
       <c r="C92" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D92" t="s">
         <v>36</v>
@@ -2922,13 +2960,13 @@
         <v>46</v>
       </c>
       <c r="F92">
-        <v>0.9638987688098496</v>
+        <v>0.93590971272229828</v>
       </c>
       <c r="G92" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>9</v>
       </c>
@@ -2936,7 +2974,7 @@
         <v>8</v>
       </c>
       <c r="C93" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D93" t="s">
         <v>36</v>
@@ -2945,13 +2983,13 @@
         <v>47</v>
       </c>
       <c r="F93">
-        <v>0.7233333333333333</v>
+        <v>0</v>
       </c>
       <c r="G93" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>9</v>
       </c>
@@ -2959,7 +2997,7 @@
         <v>8</v>
       </c>
       <c r="C94" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D94" t="s">
         <v>36</v>
@@ -2968,13 +3006,13 @@
         <v>48</v>
       </c>
       <c r="F94">
-        <v>0.6848809523809524</v>
+        <v>0</v>
       </c>
       <c r="G94" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>9</v>
       </c>
@@ -2982,206 +3020,206 @@
         <v>8</v>
       </c>
       <c r="C95" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D95" t="s">
+        <v>36</v>
+      </c>
+      <c r="E95" t="s">
+        <v>46</v>
+      </c>
+      <c r="F95">
+        <v>0.93590971272229828</v>
+      </c>
+      <c r="G95" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>9</v>
+      </c>
+      <c r="B96">
+        <v>8</v>
+      </c>
+      <c r="C96" t="s">
+        <v>11</v>
+      </c>
+      <c r="D96" t="s">
+        <v>36</v>
+      </c>
+      <c r="E96" t="s">
+        <v>47</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>9</v>
+      </c>
+      <c r="B97">
+        <v>8</v>
+      </c>
+      <c r="C97" t="s">
+        <v>11</v>
+      </c>
+      <c r="D97" t="s">
+        <v>36</v>
+      </c>
+      <c r="E97" t="s">
+        <v>48</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>9</v>
+      </c>
+      <c r="B98">
+        <v>8</v>
+      </c>
+      <c r="C98" t="s">
+        <v>18</v>
+      </c>
+      <c r="D98" t="s">
         <v>37</v>
       </c>
-      <c r="E95" t="s">
-        <v>46</v>
-      </c>
-      <c r="F95">
-        <v>0.9580437756497947</v>
-      </c>
-      <c r="G95" t="s">
+      <c r="E98" t="s">
+        <v>46</v>
+      </c>
+      <c r="F98">
+        <v>0.96504787961696292</v>
+      </c>
+      <c r="G98" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
-      <c r="A96" t="s">
-        <v>9</v>
-      </c>
-      <c r="B96">
-        <v>8</v>
-      </c>
-      <c r="C96" t="s">
-        <v>22</v>
-      </c>
-      <c r="D96" t="s">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>9</v>
+      </c>
+      <c r="B99">
+        <v>8</v>
+      </c>
+      <c r="C99" t="s">
+        <v>18</v>
+      </c>
+      <c r="D99" t="s">
         <v>37</v>
       </c>
-      <c r="E96" t="s">
-        <v>47</v>
-      </c>
-      <c r="F96">
-        <v>0.86</v>
-      </c>
-      <c r="G96" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7">
-      <c r="A97" t="s">
-        <v>9</v>
-      </c>
-      <c r="B97">
-        <v>8</v>
-      </c>
-      <c r="C97" t="s">
-        <v>22</v>
-      </c>
-      <c r="D97" t="s">
+      <c r="E99" t="s">
+        <v>47</v>
+      </c>
+      <c r="F99">
+        <v>0.67666666666666664</v>
+      </c>
+      <c r="G99" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>9</v>
+      </c>
+      <c r="B100">
+        <v>8</v>
+      </c>
+      <c r="C100" t="s">
+        <v>18</v>
+      </c>
+      <c r="D100" t="s">
         <v>37</v>
       </c>
-      <c r="E97" t="s">
-        <v>48</v>
-      </c>
-      <c r="F97">
-        <v>0.6547222222222222</v>
-      </c>
-      <c r="G97" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7">
-      <c r="A98" t="s">
-        <v>9</v>
-      </c>
-      <c r="B98">
-        <v>8</v>
-      </c>
-      <c r="C98" t="s">
-        <v>20</v>
-      </c>
-      <c r="D98" t="s">
+      <c r="E100" t="s">
+        <v>48</v>
+      </c>
+      <c r="F100">
+        <v>0.78119047619047621</v>
+      </c>
+      <c r="G100" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>9</v>
+      </c>
+      <c r="B101">
+        <v>8</v>
+      </c>
+      <c r="C101" t="s">
+        <v>16</v>
+      </c>
+      <c r="D101" t="s">
         <v>38</v>
       </c>
-      <c r="E98" t="s">
-        <v>46</v>
-      </c>
-      <c r="F98">
-        <v>0.9627086183310534</v>
-      </c>
-      <c r="G98" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7">
-      <c r="A99" t="s">
-        <v>9</v>
-      </c>
-      <c r="B99">
-        <v>8</v>
-      </c>
-      <c r="C99" t="s">
-        <v>20</v>
-      </c>
-      <c r="D99" t="s">
+      <c r="E101" t="s">
+        <v>46</v>
+      </c>
+      <c r="F101">
+        <v>0.95570451436388504</v>
+      </c>
+      <c r="G101" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>9</v>
+      </c>
+      <c r="B102">
+        <v>8</v>
+      </c>
+      <c r="C102" t="s">
+        <v>16</v>
+      </c>
+      <c r="D102" t="s">
         <v>38</v>
       </c>
-      <c r="E99" t="s">
-        <v>47</v>
-      </c>
-      <c r="F99">
-        <v>0.6366666666666667</v>
-      </c>
-      <c r="G99" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7">
-      <c r="A100" t="s">
-        <v>9</v>
-      </c>
-      <c r="B100">
-        <v>8</v>
-      </c>
-      <c r="C100" t="s">
-        <v>20</v>
-      </c>
-      <c r="D100" t="s">
+      <c r="E102" t="s">
+        <v>47</v>
+      </c>
+      <c r="F102">
+        <v>0.87666666666666671</v>
+      </c>
+      <c r="G102" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>9</v>
+      </c>
+      <c r="B103">
+        <v>8</v>
+      </c>
+      <c r="C103" t="s">
+        <v>16</v>
+      </c>
+      <c r="D103" t="s">
         <v>38</v>
       </c>
-      <c r="E100" t="s">
-        <v>48</v>
-      </c>
-      <c r="F100">
-        <v>0.7661904761904762</v>
-      </c>
-      <c r="G100" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7">
-      <c r="A101" t="s">
-        <v>9</v>
-      </c>
-      <c r="B101">
-        <v>8</v>
-      </c>
-      <c r="C101" t="s">
-        <v>19</v>
-      </c>
-      <c r="D101" t="s">
-        <v>39</v>
-      </c>
-      <c r="E101" t="s">
-        <v>46</v>
-      </c>
-      <c r="F101">
-        <v>0.9498905608755128</v>
-      </c>
-      <c r="G101" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7">
-      <c r="A102" t="s">
-        <v>9</v>
-      </c>
-      <c r="B102">
-        <v>8</v>
-      </c>
-      <c r="C102" t="s">
-        <v>19</v>
-      </c>
-      <c r="D102" t="s">
-        <v>39</v>
-      </c>
-      <c r="E102" t="s">
-        <v>47</v>
-      </c>
-      <c r="F102">
-        <v>0.7266666666666667</v>
-      </c>
-      <c r="G102" t="s">
+      <c r="E103" t="s">
+        <v>48</v>
+      </c>
+      <c r="F103">
+        <v>0.62882756132756124</v>
+      </c>
+      <c r="G103" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
-      <c r="A103" t="s">
-        <v>9</v>
-      </c>
-      <c r="B103">
-        <v>8</v>
-      </c>
-      <c r="C103" t="s">
-        <v>19</v>
-      </c>
-      <c r="D103" t="s">
-        <v>39</v>
-      </c>
-      <c r="E103" t="s">
-        <v>48</v>
-      </c>
-      <c r="F103">
-        <v>0.608452380952381</v>
-      </c>
-      <c r="G103" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>9</v>
       </c>
@@ -3192,19 +3230,19 @@
         <v>23</v>
       </c>
       <c r="D104" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E104" t="s">
         <v>46</v>
       </c>
       <c r="F104">
-        <v>0.9615595075239398</v>
+        <v>0.95221614227086193</v>
       </c>
       <c r="G104" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>9</v>
       </c>
@@ -3215,19 +3253,19 @@
         <v>23</v>
       </c>
       <c r="D105" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E105" t="s">
         <v>47</v>
       </c>
       <c r="F105">
-        <v>0.5766666666666665</v>
+        <v>0.32666666666666672</v>
       </c>
       <c r="G105" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>9</v>
       </c>
@@ -3238,19 +3276,19 @@
         <v>23</v>
       </c>
       <c r="D106" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E106" t="s">
         <v>48</v>
       </c>
       <c r="F106">
-        <v>0.7095238095238094</v>
+        <v>0.55666666666666664</v>
       </c>
       <c r="G106" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>9</v>
       </c>
@@ -3261,19 +3299,19 @@
         <v>21</v>
       </c>
       <c r="D107" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E107" t="s">
         <v>46</v>
       </c>
       <c r="F107">
-        <v>0.9603830369357045</v>
+        <v>0.96154582763337881</v>
       </c>
       <c r="G107" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>9</v>
       </c>
@@ -3284,19 +3322,19 @@
         <v>21</v>
       </c>
       <c r="D108" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E108" t="s">
         <v>47</v>
       </c>
       <c r="F108">
-        <v>0.8433333333333334</v>
+        <v>0.87666666666666659</v>
       </c>
       <c r="G108" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>9</v>
       </c>
@@ -3307,157 +3345,157 @@
         <v>21</v>
       </c>
       <c r="D109" t="s">
+        <v>40</v>
+      </c>
+      <c r="E109" t="s">
+        <v>48</v>
+      </c>
+      <c r="F109">
+        <v>0.68313492063492054</v>
+      </c>
+      <c r="G109" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>9</v>
+      </c>
+      <c r="B110">
+        <v>8</v>
+      </c>
+      <c r="C110" t="s">
+        <v>20</v>
+      </c>
+      <c r="D110" t="s">
         <v>41</v>
       </c>
-      <c r="E109" t="s">
-        <v>48</v>
-      </c>
-      <c r="F109">
-        <v>0.677579365079365</v>
-      </c>
-      <c r="G109" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7">
-      <c r="A110" t="s">
-        <v>9</v>
-      </c>
-      <c r="B110">
-        <v>8</v>
-      </c>
-      <c r="C110" t="s">
-        <v>17</v>
-      </c>
-      <c r="D110" t="s">
+      <c r="E110" t="s">
+        <v>46</v>
+      </c>
+      <c r="F110">
+        <v>0.96621067031463748</v>
+      </c>
+      <c r="G110" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>9</v>
+      </c>
+      <c r="B111">
+        <v>8</v>
+      </c>
+      <c r="C111" t="s">
+        <v>20</v>
+      </c>
+      <c r="D111" t="s">
+        <v>41</v>
+      </c>
+      <c r="E111" t="s">
+        <v>47</v>
+      </c>
+      <c r="F111">
+        <v>0.62666666666666671</v>
+      </c>
+      <c r="G111" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>9</v>
+      </c>
+      <c r="B112">
+        <v>8</v>
+      </c>
+      <c r="C112" t="s">
+        <v>20</v>
+      </c>
+      <c r="D112" t="s">
+        <v>41</v>
+      </c>
+      <c r="E112" t="s">
+        <v>48</v>
+      </c>
+      <c r="F112">
+        <v>0.73833333333333329</v>
+      </c>
+      <c r="G112" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>9</v>
+      </c>
+      <c r="B113">
+        <v>8</v>
+      </c>
+      <c r="C113" t="s">
+        <v>19</v>
+      </c>
+      <c r="D113" t="s">
         <v>42</v>
       </c>
-      <c r="E110" t="s">
-        <v>46</v>
-      </c>
-      <c r="F110">
-        <v>0.961532147742818</v>
-      </c>
-      <c r="G110" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7">
-      <c r="A111" t="s">
-        <v>9</v>
-      </c>
-      <c r="B111">
-        <v>8</v>
-      </c>
-      <c r="C111" t="s">
-        <v>17</v>
-      </c>
-      <c r="D111" t="s">
+      <c r="E113" t="s">
+        <v>46</v>
+      </c>
+      <c r="F113">
+        <v>0.95570451436388504</v>
+      </c>
+      <c r="G113" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>9</v>
+      </c>
+      <c r="B114">
+        <v>8</v>
+      </c>
+      <c r="C114" t="s">
+        <v>19</v>
+      </c>
+      <c r="D114" t="s">
         <v>42</v>
       </c>
-      <c r="E111" t="s">
-        <v>47</v>
-      </c>
-      <c r="F111">
-        <v>0.5766666666666667</v>
-      </c>
-      <c r="G111" t="s">
+      <c r="E114" t="s">
+        <v>47</v>
+      </c>
+      <c r="F114">
+        <v>0.66999999999999993</v>
+      </c>
+      <c r="G114" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
-      <c r="A112" t="s">
-        <v>9</v>
-      </c>
-      <c r="B112">
-        <v>8</v>
-      </c>
-      <c r="C112" t="s">
-        <v>17</v>
-      </c>
-      <c r="D112" t="s">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>9</v>
+      </c>
+      <c r="B115">
+        <v>8</v>
+      </c>
+      <c r="C115" t="s">
+        <v>19</v>
+      </c>
+      <c r="D115" t="s">
         <v>42</v>
       </c>
-      <c r="E112" t="s">
-        <v>48</v>
-      </c>
-      <c r="F112">
-        <v>0.7533333333333333</v>
-      </c>
-      <c r="G112" t="s">
+      <c r="E115" t="s">
+        <v>48</v>
+      </c>
+      <c r="F115">
+        <v>0.67154761904761906</v>
+      </c>
+      <c r="G115" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
-      <c r="A113" t="s">
-        <v>9</v>
-      </c>
-      <c r="B113">
-        <v>8</v>
-      </c>
-      <c r="C113" t="s">
-        <v>15</v>
-      </c>
-      <c r="D113" t="s">
-        <v>36</v>
-      </c>
-      <c r="E113" t="s">
-        <v>46</v>
-      </c>
-      <c r="F113">
-        <v>0.953392612859097</v>
-      </c>
-      <c r="G113" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7">
-      <c r="A114" t="s">
-        <v>9</v>
-      </c>
-      <c r="B114">
-        <v>8</v>
-      </c>
-      <c r="C114" t="s">
-        <v>15</v>
-      </c>
-      <c r="D114" t="s">
-        <v>36</v>
-      </c>
-      <c r="E114" t="s">
-        <v>47</v>
-      </c>
-      <c r="F114">
-        <v>0.8</v>
-      </c>
-      <c r="G114" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7">
-      <c r="A115" t="s">
-        <v>9</v>
-      </c>
-      <c r="B115">
-        <v>8</v>
-      </c>
-      <c r="C115" t="s">
-        <v>15</v>
-      </c>
-      <c r="D115" t="s">
-        <v>36</v>
-      </c>
-      <c r="E115" t="s">
-        <v>48</v>
-      </c>
-      <c r="F115">
-        <v>0.6361688311688312</v>
-      </c>
-      <c r="G115" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>9</v>
       </c>
@@ -3465,7 +3503,7 @@
         <v>8</v>
       </c>
       <c r="C116" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D116" t="s">
         <v>43</v>
@@ -3474,13 +3512,13 @@
         <v>46</v>
       </c>
       <c r="F116">
-        <v>0.9592065663474691</v>
+        <v>0.93707250341997261</v>
       </c>
       <c r="G116" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>9</v>
       </c>
@@ -3488,7 +3526,7 @@
         <v>8</v>
       </c>
       <c r="C117" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D117" t="s">
         <v>43</v>
@@ -3497,13 +3535,13 @@
         <v>47</v>
       </c>
       <c r="F117">
-        <v>0.6566666666666667</v>
+        <v>0.04</v>
       </c>
       <c r="G117" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>9</v>
       </c>
@@ -3511,7 +3549,7 @@
         <v>8</v>
       </c>
       <c r="C118" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D118" t="s">
         <v>43</v>
@@ -3520,13 +3558,13 @@
         <v>48</v>
       </c>
       <c r="F118">
-        <v>0.6933333333333334</v>
+        <v>0.15</v>
       </c>
       <c r="G118" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>9</v>
       </c>
@@ -3534,22 +3572,22 @@
         <v>8</v>
       </c>
       <c r="C119" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D119" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E119" t="s">
         <v>46</v>
       </c>
       <c r="F119">
-        <v>0.9521887824897399</v>
+        <v>0.93590971272229828</v>
       </c>
       <c r="G119" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>9</v>
       </c>
@@ -3557,22 +3595,22 @@
         <v>8</v>
       </c>
       <c r="C120" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D120" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E120" t="s">
         <v>47</v>
       </c>
       <c r="F120">
-        <v>0.7666666666666666</v>
+        <v>0</v>
       </c>
       <c r="G120" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>9</v>
       </c>
@@ -3580,22 +3618,22 @@
         <v>8</v>
       </c>
       <c r="C121" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D121" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E121" t="s">
         <v>48</v>
       </c>
       <c r="F121">
-        <v>0.6270238095238094</v>
+        <v>0</v>
       </c>
       <c r="G121" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>9</v>
       </c>
@@ -3603,22 +3641,22 @@
         <v>10</v>
       </c>
       <c r="C122" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D122" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E122" t="s">
         <v>46</v>
       </c>
       <c r="F122">
-        <v>0.9359097127222983</v>
+        <v>0.96621067031463748</v>
       </c>
       <c r="G122" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>9</v>
       </c>
@@ -3626,22 +3664,22 @@
         <v>10</v>
       </c>
       <c r="C123" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D123" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E123" t="s">
         <v>47</v>
       </c>
       <c r="F123">
-        <v>0</v>
+        <v>0.76999999999999991</v>
       </c>
       <c r="G123" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>9</v>
       </c>
@@ -3649,22 +3687,22 @@
         <v>10</v>
       </c>
       <c r="C124" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D124" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E124" t="s">
         <v>48</v>
       </c>
       <c r="F124">
-        <v>0</v>
+        <v>0.74821428571428572</v>
       </c>
       <c r="G124" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>9</v>
       </c>
@@ -3672,7 +3710,7 @@
         <v>10</v>
       </c>
       <c r="C125" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D125" t="s">
         <v>45</v>
@@ -3681,13 +3719,13 @@
         <v>46</v>
       </c>
       <c r="F125">
-        <v>0.6831053351573189</v>
+        <v>0.96154582763337881</v>
       </c>
       <c r="G125" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>9</v>
       </c>
@@ -3695,7 +3733,7 @@
         <v>10</v>
       </c>
       <c r="C126" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D126" t="s">
         <v>45</v>
@@ -3704,13 +3742,13 @@
         <v>47</v>
       </c>
       <c r="F126">
-        <v>0.2466666666666666</v>
+        <v>0.87666666666666659</v>
       </c>
       <c r="G126" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>9</v>
       </c>
@@ -3718,7 +3756,7 @@
         <v>10</v>
       </c>
       <c r="C127" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D127" t="s">
         <v>45</v>
@@ -3727,10 +3765,10 @@
         <v>48</v>
       </c>
       <c r="F127">
-        <v>0.05965825439738483</v>
+        <v>0.68313492063492054</v>
       </c>
       <c r="G127" t="s">
-        <v>144</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atividade 9 - Random Forests
</commit_message>
<xml_diff>
--- a/model_results/all_models_results.xlsx
+++ b/model_results/all_models_results.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LHS\Documents\GitHub\projeto_SIN5007_rec_padroes\model_results\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155AF734-F489-4FA9-82F1-0D12B7DBF3A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="147">
   <si>
     <t>Algoritmo</t>
   </si>
@@ -52,7 +46,10 @@
     <t>MLPClassifier</t>
   </si>
   <si>
-    <t>8</t>
+    <t>RandomForestClassifier</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
   <si>
     <t>Branch and Bound Balanceado - Nao Normalizado</t>
@@ -160,6 +157,12 @@
     <t>((7,), 0.001, 'tanh', 0.6, 300, False)</t>
   </si>
   <si>
+    <t>('log2', 800)</t>
+  </si>
+  <si>
+    <t>('log2', 600)</t>
+  </si>
+  <si>
     <t>Accuracy</t>
   </si>
   <si>
@@ -437,13 +440,28 @@
   </si>
   <si>
     <t>[0.748, 0.600, 0.896]</t>
+  </si>
+  <si>
+    <t>[0.958, 0.944, 0.972]</t>
+  </si>
+  <si>
+    <t>[0.627, 0.503, 0.750]</t>
+  </si>
+  <si>
+    <t>[0.727, 0.596, 0.857]</t>
+  </si>
+  <si>
+    <t>[0.777, 0.618, 0.935]</t>
+  </si>
+  <si>
+    <t>[0.686, 0.558, 0.815]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -506,14 +524,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -560,7 +570,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -592,27 +602,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -644,24 +636,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -837,20 +811,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G127"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="A127" sqref="A86:XFD127"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="47.5703125" customWidth="1"/>
-    <col min="4" max="4" width="64.85546875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -873,7 +841,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -881,22 +849,22 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F2">
-        <v>0.89612859097127218</v>
+        <v>0.8961285909712722</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -904,22 +872,22 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F3">
         <v>0.02</v>
       </c>
       <c r="G3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -927,22 +895,22 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F4">
-        <v>6.666666666666668E-3</v>
+        <v>0.006666666666666668</v>
       </c>
       <c r="G4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -950,22 +918,22 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <v>0.3</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F5">
-        <v>0.69010943912448686</v>
+        <v>0.6901094391244869</v>
       </c>
       <c r="G5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -973,22 +941,22 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>0.3</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F6">
         <v>0.2166666666666667</v>
       </c>
       <c r="G6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -996,22 +964,22 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <v>0.3</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F7">
-        <v>4.9271192942079017E-2</v>
+        <v>0.04927119294207902</v>
       </c>
       <c r="G7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1019,22 +987,22 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F8">
-        <v>0.82288645690834472</v>
+        <v>0.8228864569083447</v>
       </c>
       <c r="G8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1042,22 +1010,22 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F9">
-        <v>0.15333333333333329</v>
+        <v>0.1533333333333333</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1065,22 +1033,22 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F10">
-        <v>9.0642135642135649E-2</v>
+        <v>0.09064213564213565</v>
       </c>
       <c r="G10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1088,22 +1056,22 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D11">
         <v>0.1</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F11">
         <v>0.5128454172366621</v>
       </c>
       <c r="G11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1111,22 +1079,22 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D12">
         <v>0.1</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F12">
         <v>0.5033333333333333</v>
       </c>
       <c r="G12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1134,22 +1102,22 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13">
         <v>0.1</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F13">
-        <v>6.7476424659444562E-2</v>
+        <v>0.06747642465944456</v>
       </c>
       <c r="G13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1157,22 +1125,22 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F14">
-        <v>0.93823529411764695</v>
+        <v>0.9382352941176469</v>
       </c>
       <c r="G14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1180,22 +1148,22 @@
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F15">
-        <v>8.3333333333333329E-2</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="G15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1203,22 +1171,22 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F16">
         <v>0.35</v>
       </c>
       <c r="G16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1226,22 +1194,22 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D17">
         <v>0.6</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F17">
-        <v>0.93124487004103962</v>
+        <v>0.9312448700410396</v>
       </c>
       <c r="G17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1249,22 +1217,22 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D18">
         <v>0.6</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1272,22 +1240,22 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D19">
         <v>0.6</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1295,22 +1263,22 @@
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F20">
-        <v>0.93590971272229828</v>
+        <v>0.9359097127222983</v>
       </c>
       <c r="G20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1318,22 +1286,22 @@
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1341,22 +1309,22 @@
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E22" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1364,22 +1332,22 @@
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F23">
         <v>0.9300547195622435</v>
       </c>
       <c r="G23" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1387,22 +1355,22 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F24">
         <v>0.02</v>
       </c>
       <c r="G24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1410,22 +1378,22 @@
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F25">
         <v>0.1</v>
       </c>
       <c r="G25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1433,22 +1401,22 @@
         <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E26" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F26">
-        <v>0.96270861833105337</v>
+        <v>0.9627086183310534</v>
       </c>
       <c r="G26" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1456,22 +1424,22 @@
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E27" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F27">
-        <v>0.87666666666666659</v>
+        <v>0.8766666666666666</v>
       </c>
       <c r="G27" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1479,22 +1447,22 @@
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E28" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F28">
-        <v>0.69007936507936507</v>
+        <v>0.6900793650793651</v>
       </c>
       <c r="G28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1502,22 +1470,22 @@
         <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D29">
         <v>0.8</v>
       </c>
       <c r="E29" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F29">
-        <v>0.93932968536251715</v>
+        <v>0.9393296853625172</v>
       </c>
       <c r="G29" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1525,22 +1493,22 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D30">
         <v>0.8</v>
       </c>
       <c r="E30" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F30">
-        <v>0.87666666666666659</v>
+        <v>0.8766666666666666</v>
       </c>
       <c r="G30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1548,22 +1516,22 @@
         <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D31">
         <v>0.8</v>
       </c>
       <c r="E31" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F31">
-        <v>0.54714285714285704</v>
+        <v>0.547142857142857</v>
       </c>
       <c r="G31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1571,22 +1539,22 @@
         <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D32" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E32" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F32">
-        <v>0.95919288645690826</v>
+        <v>0.9591928864569083</v>
       </c>
       <c r="G32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -1594,22 +1562,22 @@
         <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D33" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E33" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F33">
-        <v>0.91000000000000014</v>
+        <v>0.9100000000000001</v>
       </c>
       <c r="G33" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -1617,22 +1585,22 @@
         <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D34" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E34" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F34">
-        <v>0.67301587301587307</v>
+        <v>0.6730158730158731</v>
       </c>
       <c r="G34" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -1640,22 +1608,22 @@
         <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D35">
         <v>0.2</v>
       </c>
       <c r="E35" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F35">
-        <v>0.93584131326949382</v>
+        <v>0.9358413132694938</v>
       </c>
       <c r="G35" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -1663,22 +1631,22 @@
         <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D36">
         <v>0.2</v>
       </c>
       <c r="E36" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F36">
-        <v>0.87666666666666659</v>
+        <v>0.8766666666666666</v>
       </c>
       <c r="G36" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -1686,22 +1654,22 @@
         <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D37">
         <v>0.2</v>
       </c>
       <c r="E37" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F37">
-        <v>0.52769841269841267</v>
+        <v>0.5276984126984127</v>
       </c>
       <c r="G37" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -1709,22 +1677,22 @@
         <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D38" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E38" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F38">
-        <v>0.96038303693570448</v>
+        <v>0.9603830369357045</v>
       </c>
       <c r="G38" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1732,22 +1700,22 @@
         <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D39" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E39" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F39">
         <v>0.86</v>
       </c>
       <c r="G39" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -1755,22 +1723,22 @@
         <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E40" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F40">
         <v>0.677579365079365</v>
       </c>
       <c r="G40" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -1778,22 +1746,22 @@
         <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D41">
         <v>0.6</v>
       </c>
       <c r="E41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F41">
-        <v>0.95567715458276337</v>
+        <v>0.9556771545827634</v>
       </c>
       <c r="G41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -1801,22 +1769,22 @@
         <v>6</v>
       </c>
       <c r="C42" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D42">
         <v>0.6</v>
       </c>
       <c r="E42" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F42">
-        <v>0.71666666666666656</v>
+        <v>0.7166666666666666</v>
       </c>
       <c r="G42" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -1824,22 +1792,22 @@
         <v>6</v>
       </c>
       <c r="C43" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D43">
         <v>0.6</v>
       </c>
       <c r="E43" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F43">
-        <v>0.67539682539682544</v>
+        <v>0.6753968253968254</v>
       </c>
       <c r="G43" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -1847,22 +1815,22 @@
         <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D44" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E44" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F44">
-        <v>0.96270861833105337</v>
+        <v>0.9627086183310534</v>
       </c>
       <c r="G44" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -1870,22 +1838,22 @@
         <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D45" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E45" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F45">
-        <v>0.87666666666666659</v>
+        <v>0.8766666666666666</v>
       </c>
       <c r="G45" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -1893,22 +1861,22 @@
         <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D46" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E46" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F46">
-        <v>0.69007936507936507</v>
+        <v>0.6900793650793651</v>
       </c>
       <c r="G46" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -1916,22 +1884,22 @@
         <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D47">
         <v>0.9</v>
       </c>
       <c r="E47" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F47">
-        <v>0.94753761969904249</v>
+        <v>0.9475376196990425</v>
       </c>
       <c r="G47" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -1939,22 +1907,22 @@
         <v>6</v>
       </c>
       <c r="C48" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D48">
         <v>0.9</v>
       </c>
       <c r="E48" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F48">
-        <v>0.71666666666666656</v>
+        <v>0.7166666666666666</v>
       </c>
       <c r="G48" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -1962,22 +1930,22 @@
         <v>6</v>
       </c>
       <c r="C49" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D49">
         <v>0.9</v>
       </c>
       <c r="E49" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F49">
-        <v>0.60444444444444445</v>
+        <v>0.6044444444444445</v>
       </c>
       <c r="G49" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -1985,22 +1953,22 @@
         <v>7</v>
       </c>
       <c r="C50" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D50" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E50" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F50">
         <v>0.9580574555403556</v>
       </c>
       <c r="G50" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -2008,22 +1976,22 @@
         <v>7</v>
       </c>
       <c r="C51" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D51" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E51" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F51">
-        <v>0.71666666666666656</v>
+        <v>0.7166666666666666</v>
       </c>
       <c r="G51" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -2031,22 +1999,22 @@
         <v>7</v>
       </c>
       <c r="C52" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D52" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E52" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F52">
-        <v>0.71380952380952378</v>
+        <v>0.7138095238095238</v>
       </c>
       <c r="G52" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -2054,22 +2022,22 @@
         <v>6</v>
       </c>
       <c r="C53" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F53">
-        <v>0.94169630642954849</v>
+        <v>0.9416963064295485</v>
       </c>
       <c r="G53" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -2077,22 +2045,22 @@
         <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D54">
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F54">
         <v>0.64</v>
       </c>
       <c r="G54" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>8</v>
       </c>
@@ -2100,22 +2068,22 @@
         <v>6</v>
       </c>
       <c r="C55" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D55">
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F55">
-        <v>0.57047619047619047</v>
+        <v>0.5704761904761905</v>
       </c>
       <c r="G55" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -2123,22 +2091,22 @@
         <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D56" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E56" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F56">
-        <v>0.96389876880984937</v>
+        <v>0.9638987688098494</v>
       </c>
       <c r="G56" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -2146,22 +2114,22 @@
         <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D57" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E57" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F57">
         <v>0.6399999999999999</v>
       </c>
       <c r="G57" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -2169,22 +2137,22 @@
         <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D58" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E58" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F58">
-        <v>0.79952380952380953</v>
+        <v>0.7995238095238095</v>
       </c>
       <c r="G58" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -2192,22 +2160,22 @@
         <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D59">
         <v>0.9</v>
       </c>
       <c r="E59" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F59">
-        <v>0.93355677154582772</v>
+        <v>0.9335567715458277</v>
       </c>
       <c r="G59" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -2215,22 +2183,22 @@
         <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D60">
         <v>0.9</v>
       </c>
       <c r="E60" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F60">
         <v>0.11</v>
       </c>
       <c r="G60" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -2238,22 +2206,22 @@
         <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D61">
         <v>0.9</v>
       </c>
       <c r="E61" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F61">
-        <v>0.21666666666666659</v>
+        <v>0.2166666666666666</v>
       </c>
       <c r="G61" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" t="s">
         <v>7</v>
       </c>
@@ -2261,22 +2229,22 @@
         <v>7</v>
       </c>
       <c r="C62" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D62" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E62" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F62">
-        <v>0.96270861833105337</v>
+        <v>0.9627086183310534</v>
       </c>
       <c r="G62" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" t="s">
         <v>7</v>
       </c>
@@ -2284,22 +2252,22 @@
         <v>7</v>
       </c>
       <c r="C63" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D63" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E63" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F63">
-        <v>0.87666666666666659</v>
+        <v>0.8766666666666666</v>
       </c>
       <c r="G63" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" t="s">
         <v>7</v>
       </c>
@@ -2307,22 +2275,22 @@
         <v>7</v>
       </c>
       <c r="C64" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D64" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E64" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F64">
-        <v>0.69007936507936507</v>
+        <v>0.6900793650793651</v>
       </c>
       <c r="G64" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
         <v>8</v>
       </c>
@@ -2330,22 +2298,22 @@
         <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D65">
         <v>0.1</v>
       </c>
       <c r="E65" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F65">
-        <v>0.95689466484268126</v>
+        <v>0.9568946648426813</v>
       </c>
       <c r="G65" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -2353,22 +2321,22 @@
         <v>6</v>
       </c>
       <c r="C66" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D66">
         <v>0.1</v>
       </c>
       <c r="E66" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F66">
-        <v>0.87666666666666659</v>
+        <v>0.8766666666666666</v>
       </c>
       <c r="G66" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" t="s">
         <v>8</v>
       </c>
@@ -2376,22 +2344,22 @@
         <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D67">
         <v>0.1</v>
       </c>
       <c r="E67" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F67">
-        <v>0.65230158730158727</v>
+        <v>0.6523015873015873</v>
       </c>
       <c r="G67" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -2399,22 +2367,22 @@
         <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D68" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E68" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F68">
         <v>0.9638714090287277</v>
       </c>
       <c r="G68" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" t="s">
         <v>7</v>
       </c>
@@ -2422,22 +2390,22 @@
         <v>7</v>
       </c>
       <c r="C69" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D69" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E69" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F69">
-        <v>0.87666666666666659</v>
+        <v>0.8766666666666666</v>
       </c>
       <c r="G69" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
         <v>7</v>
       </c>
@@ -2445,22 +2413,22 @@
         <v>7</v>
       </c>
       <c r="C70" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D70" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E70" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F70">
-        <v>0.69722222222222219</v>
+        <v>0.6972222222222222</v>
       </c>
       <c r="G70" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" t="s">
         <v>8</v>
       </c>
@@ -2468,22 +2436,22 @@
         <v>6</v>
       </c>
       <c r="C71" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D71">
         <v>0.2</v>
       </c>
       <c r="E71" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F71">
-        <v>0.95689466484268126</v>
+        <v>0.9568946648426813</v>
       </c>
       <c r="G71" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72" t="s">
         <v>8</v>
       </c>
@@ -2491,22 +2459,22 @@
         <v>6</v>
       </c>
       <c r="C72" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D72">
         <v>0.2</v>
       </c>
       <c r="E72" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F72">
-        <v>0.87666666666666659</v>
+        <v>0.8766666666666666</v>
       </c>
       <c r="G72" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" t="s">
         <v>8</v>
       </c>
@@ -2514,22 +2482,22 @@
         <v>6</v>
       </c>
       <c r="C73" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D73">
         <v>0.2</v>
       </c>
       <c r="E73" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F73">
-        <v>0.65230158730158727</v>
+        <v>0.6523015873015873</v>
       </c>
       <c r="G73" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74" t="s">
         <v>7</v>
       </c>
@@ -2537,22 +2505,22 @@
         <v>7</v>
       </c>
       <c r="C74" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D74" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E74" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F74">
-        <v>0.96154582763337881</v>
+        <v>0.9615458276333788</v>
       </c>
       <c r="G74" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75" t="s">
         <v>7</v>
       </c>
@@ -2560,22 +2528,22 @@
         <v>7</v>
       </c>
       <c r="C75" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D75" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E75" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F75">
-        <v>0.87666666666666659</v>
+        <v>0.8766666666666666</v>
       </c>
       <c r="G75" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76" t="s">
         <v>7</v>
       </c>
@@ -2583,22 +2551,22 @@
         <v>7</v>
       </c>
       <c r="C76" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D76" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E76" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F76">
-        <v>0.68313492063492054</v>
+        <v>0.6831349206349205</v>
       </c>
       <c r="G76" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" t="s">
         <v>8</v>
       </c>
@@ -2606,22 +2574,22 @@
         <v>6</v>
       </c>
       <c r="C77" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D77">
         <v>0.4</v>
       </c>
       <c r="E77" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F77">
-        <v>0.96272229822161415</v>
+        <v>0.9627222982216141</v>
       </c>
       <c r="G77" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78" t="s">
         <v>8</v>
       </c>
@@ -2629,22 +2597,22 @@
         <v>6</v>
       </c>
       <c r="C78" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D78">
         <v>0.4</v>
       </c>
       <c r="E78" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F78">
-        <v>0.69666666666666666</v>
+        <v>0.6966666666666667</v>
       </c>
       <c r="G78" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79" t="s">
         <v>8</v>
       </c>
@@ -2652,22 +2620,22 @@
         <v>6</v>
       </c>
       <c r="C79" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D79">
         <v>0.4</v>
       </c>
       <c r="E79" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F79">
-        <v>0.75380952380952393</v>
+        <v>0.7538095238095239</v>
       </c>
       <c r="G79" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80" t="s">
         <v>7</v>
       </c>
@@ -2675,22 +2643,22 @@
         <v>7</v>
       </c>
       <c r="C80" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D80" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E80" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F80">
-        <v>0.96154582763337904</v>
+        <v>0.961545827633379</v>
       </c>
       <c r="G80" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" t="s">
         <v>7</v>
       </c>
@@ -2698,22 +2666,22 @@
         <v>7</v>
       </c>
       <c r="C81" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D81" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E81" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F81">
-        <v>0.65999999999999992</v>
+        <v>0.6599999999999999</v>
       </c>
       <c r="G81" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" t="s">
         <v>7</v>
       </c>
@@ -2721,22 +2689,22 @@
         <v>7</v>
       </c>
       <c r="C82" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D82" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E82" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F82">
-        <v>0.73666666666666658</v>
+        <v>0.7366666666666666</v>
       </c>
       <c r="G82" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" t="s">
         <v>8</v>
       </c>
@@ -2744,22 +2712,22 @@
         <v>6</v>
       </c>
       <c r="C83" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D83">
         <v>0.8</v>
       </c>
       <c r="E83" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F83">
-        <v>0.96272229822161415</v>
+        <v>0.9627222982216141</v>
       </c>
       <c r="G83" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84" t="s">
         <v>8</v>
       </c>
@@ -2767,22 +2735,22 @@
         <v>6</v>
       </c>
       <c r="C84" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D84">
         <v>0.8</v>
       </c>
       <c r="E84" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F84">
-        <v>0.69666666666666666</v>
+        <v>0.6966666666666667</v>
       </c>
       <c r="G84" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" t="s">
         <v>8</v>
       </c>
@@ -2790,22 +2758,22 @@
         <v>6</v>
       </c>
       <c r="C85" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D85">
         <v>0.8</v>
       </c>
       <c r="E85" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F85">
-        <v>0.75380952380952393</v>
+        <v>0.7538095238095239</v>
       </c>
       <c r="G85" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86" t="s">
         <v>9</v>
       </c>
@@ -2813,22 +2781,22 @@
         <v>8</v>
       </c>
       <c r="C86" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D86" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E86" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F86">
-        <v>0.95570451436388504</v>
+        <v>0.955704514363885</v>
       </c>
       <c r="G86" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87" t="s">
         <v>9</v>
       </c>
@@ -2836,22 +2804,22 @@
         <v>8</v>
       </c>
       <c r="C87" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D87" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E87" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F87">
-        <v>0.59666666666666668</v>
+        <v>0.5966666666666667</v>
       </c>
       <c r="G87" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88" t="s">
         <v>9</v>
       </c>
@@ -2859,22 +2827,22 @@
         <v>8</v>
       </c>
       <c r="C88" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D88" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E88" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F88">
-        <v>0.69261904761904758</v>
+        <v>0.6926190476190476</v>
       </c>
       <c r="G88" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89" t="s">
         <v>9</v>
       </c>
@@ -2882,22 +2850,22 @@
         <v>8</v>
       </c>
       <c r="C89" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D89" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E89" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F89">
-        <v>0.95801641586867292</v>
+        <v>0.9580164158686729</v>
       </c>
       <c r="G89" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90" t="s">
         <v>9</v>
       </c>
@@ -2905,22 +2873,22 @@
         <v>8</v>
       </c>
       <c r="C90" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D90" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E90" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F90">
-        <v>0.84000000000000008</v>
+        <v>0.8400000000000001</v>
       </c>
       <c r="G90" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" t="s">
         <v>9</v>
       </c>
@@ -2928,22 +2896,22 @@
         <v>8</v>
       </c>
       <c r="C91" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D91" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E91" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F91">
-        <v>0.66731601731601731</v>
+        <v>0.6673160173160173</v>
       </c>
       <c r="G91" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92" t="s">
         <v>9</v>
       </c>
@@ -2951,22 +2919,22 @@
         <v>8</v>
       </c>
       <c r="C92" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D92" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E92" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F92">
-        <v>0.93590971272229828</v>
+        <v>0.9359097127222983</v>
       </c>
       <c r="G92" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93" t="s">
         <v>9</v>
       </c>
@@ -2974,22 +2942,22 @@
         <v>8</v>
       </c>
       <c r="C93" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D93" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E93" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F93">
         <v>0</v>
       </c>
       <c r="G93" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94" t="s">
         <v>9</v>
       </c>
@@ -2997,22 +2965,22 @@
         <v>8</v>
       </c>
       <c r="C94" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D94" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E94" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F94">
         <v>0</v>
       </c>
       <c r="G94" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95" t="s">
         <v>9</v>
       </c>
@@ -3020,22 +2988,22 @@
         <v>8</v>
       </c>
       <c r="C95" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D95" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E95" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F95">
-        <v>0.93590971272229828</v>
+        <v>0.9359097127222983</v>
       </c>
       <c r="G95" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96" t="s">
         <v>9</v>
       </c>
@@ -3043,22 +3011,22 @@
         <v>8</v>
       </c>
       <c r="C96" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D96" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E96" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F96">
         <v>0</v>
       </c>
       <c r="G96" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
       <c r="A97" t="s">
         <v>9</v>
       </c>
@@ -3066,22 +3034,22 @@
         <v>8</v>
       </c>
       <c r="C97" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D97" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E97" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F97">
         <v>0</v>
       </c>
       <c r="G97" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
       <c r="A98" t="s">
         <v>9</v>
       </c>
@@ -3089,22 +3057,22 @@
         <v>8</v>
       </c>
       <c r="C98" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D98" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E98" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F98">
-        <v>0.96504787961696292</v>
+        <v>0.9650478796169629</v>
       </c>
       <c r="G98" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
       <c r="A99" t="s">
         <v>9</v>
       </c>
@@ -3112,22 +3080,22 @@
         <v>8</v>
       </c>
       <c r="C99" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D99" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E99" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F99">
-        <v>0.67666666666666664</v>
+        <v>0.6766666666666666</v>
       </c>
       <c r="G99" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
       <c r="A100" t="s">
         <v>9</v>
       </c>
@@ -3135,22 +3103,22 @@
         <v>8</v>
       </c>
       <c r="C100" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D100" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E100" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F100">
-        <v>0.78119047619047621</v>
+        <v>0.7811904761904762</v>
       </c>
       <c r="G100" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
       <c r="A101" t="s">
         <v>9</v>
       </c>
@@ -3158,22 +3126,22 @@
         <v>8</v>
       </c>
       <c r="C101" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D101" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E101" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F101">
-        <v>0.95570451436388504</v>
+        <v>0.955704514363885</v>
       </c>
       <c r="G101" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
       <c r="A102" t="s">
         <v>9</v>
       </c>
@@ -3181,22 +3149,22 @@
         <v>8</v>
       </c>
       <c r="C102" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D102" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E102" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F102">
-        <v>0.87666666666666671</v>
+        <v>0.8766666666666667</v>
       </c>
       <c r="G102" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
       <c r="A103" t="s">
         <v>9</v>
       </c>
@@ -3204,22 +3172,22 @@
         <v>8</v>
       </c>
       <c r="C103" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D103" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E103" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F103">
-        <v>0.62882756132756124</v>
+        <v>0.6288275613275612</v>
       </c>
       <c r="G103" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
       <c r="A104" t="s">
         <v>9</v>
       </c>
@@ -3227,275 +3195,275 @@
         <v>8</v>
       </c>
       <c r="C104" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D104" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E104" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F104">
-        <v>0.95221614227086193</v>
+        <v>0.9522161422708619</v>
       </c>
       <c r="G104" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" t="s">
+        <v>9</v>
+      </c>
+      <c r="B105">
+        <v>8</v>
+      </c>
+      <c r="C105" t="s">
+        <v>24</v>
+      </c>
+      <c r="D105" t="s">
+        <v>40</v>
+      </c>
+      <c r="E105" t="s">
+        <v>50</v>
+      </c>
+      <c r="F105">
+        <v>0.3266666666666667</v>
+      </c>
+      <c r="G105" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" t="s">
+        <v>9</v>
+      </c>
+      <c r="B106">
+        <v>8</v>
+      </c>
+      <c r="C106" t="s">
+        <v>24</v>
+      </c>
+      <c r="D106" t="s">
+        <v>40</v>
+      </c>
+      <c r="E106" t="s">
+        <v>51</v>
+      </c>
+      <c r="F106">
+        <v>0.5566666666666666</v>
+      </c>
+      <c r="G106" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" t="s">
+        <v>9</v>
+      </c>
+      <c r="B107">
+        <v>8</v>
+      </c>
+      <c r="C107" t="s">
+        <v>22</v>
+      </c>
+      <c r="D107" t="s">
+        <v>41</v>
+      </c>
+      <c r="E107" t="s">
+        <v>49</v>
+      </c>
+      <c r="F107">
+        <v>0.9615458276333788</v>
+      </c>
+      <c r="G107" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" t="s">
+        <v>9</v>
+      </c>
+      <c r="B108">
+        <v>8</v>
+      </c>
+      <c r="C108" t="s">
+        <v>22</v>
+      </c>
+      <c r="D108" t="s">
+        <v>41</v>
+      </c>
+      <c r="E108" t="s">
+        <v>50</v>
+      </c>
+      <c r="F108">
+        <v>0.8766666666666666</v>
+      </c>
+      <c r="G108" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="A109" t="s">
+        <v>9</v>
+      </c>
+      <c r="B109">
+        <v>8</v>
+      </c>
+      <c r="C109" t="s">
+        <v>22</v>
+      </c>
+      <c r="D109" t="s">
+        <v>41</v>
+      </c>
+      <c r="E109" t="s">
+        <v>51</v>
+      </c>
+      <c r="F109">
+        <v>0.6831349206349205</v>
+      </c>
+      <c r="G109" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" t="s">
+        <v>9</v>
+      </c>
+      <c r="B110">
+        <v>8</v>
+      </c>
+      <c r="C110" t="s">
+        <v>21</v>
+      </c>
+      <c r="D110" t="s">
+        <v>42</v>
+      </c>
+      <c r="E110" t="s">
+        <v>49</v>
+      </c>
+      <c r="F110">
+        <v>0.9662106703146375</v>
+      </c>
+      <c r="G110" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" t="s">
+        <v>9</v>
+      </c>
+      <c r="B111">
+        <v>8</v>
+      </c>
+      <c r="C111" t="s">
+        <v>21</v>
+      </c>
+      <c r="D111" t="s">
+        <v>42</v>
+      </c>
+      <c r="E111" t="s">
+        <v>50</v>
+      </c>
+      <c r="F111">
+        <v>0.6266666666666667</v>
+      </c>
+      <c r="G111" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" t="s">
+        <v>9</v>
+      </c>
+      <c r="B112">
+        <v>8</v>
+      </c>
+      <c r="C112" t="s">
+        <v>21</v>
+      </c>
+      <c r="D112" t="s">
+        <v>42</v>
+      </c>
+      <c r="E112" t="s">
+        <v>51</v>
+      </c>
+      <c r="F112">
+        <v>0.7383333333333333</v>
+      </c>
+      <c r="G112" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" t="s">
+        <v>9</v>
+      </c>
+      <c r="B113">
+        <v>8</v>
+      </c>
+      <c r="C113" t="s">
+        <v>20</v>
+      </c>
+      <c r="D113" t="s">
+        <v>43</v>
+      </c>
+      <c r="E113" t="s">
+        <v>49</v>
+      </c>
+      <c r="F113">
+        <v>0.955704514363885</v>
+      </c>
+      <c r="G113" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>9</v>
-      </c>
-      <c r="B105">
-        <v>8</v>
-      </c>
-      <c r="C105" t="s">
-        <v>23</v>
-      </c>
-      <c r="D105" t="s">
-        <v>39</v>
-      </c>
-      <c r="E105" t="s">
-        <v>47</v>
-      </c>
-      <c r="F105">
-        <v>0.32666666666666672</v>
-      </c>
-      <c r="G105" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>9</v>
-      </c>
-      <c r="B106">
-        <v>8</v>
-      </c>
-      <c r="C106" t="s">
-        <v>23</v>
-      </c>
-      <c r="D106" t="s">
-        <v>39</v>
-      </c>
-      <c r="E106" t="s">
-        <v>48</v>
-      </c>
-      <c r="F106">
-        <v>0.55666666666666664</v>
-      </c>
-      <c r="G106" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>9</v>
-      </c>
-      <c r="B107">
-        <v>8</v>
-      </c>
-      <c r="C107" t="s">
-        <v>21</v>
-      </c>
-      <c r="D107" t="s">
-        <v>40</v>
-      </c>
-      <c r="E107" t="s">
-        <v>46</v>
-      </c>
-      <c r="F107">
-        <v>0.96154582763337881</v>
-      </c>
-      <c r="G107" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>9</v>
-      </c>
-      <c r="B108">
-        <v>8</v>
-      </c>
-      <c r="C108" t="s">
-        <v>21</v>
-      </c>
-      <c r="D108" t="s">
-        <v>40</v>
-      </c>
-      <c r="E108" t="s">
-        <v>47</v>
-      </c>
-      <c r="F108">
-        <v>0.87666666666666659</v>
-      </c>
-      <c r="G108" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>9</v>
-      </c>
-      <c r="B109">
-        <v>8</v>
-      </c>
-      <c r="C109" t="s">
-        <v>21</v>
-      </c>
-      <c r="D109" t="s">
-        <v>40</v>
-      </c>
-      <c r="E109" t="s">
-        <v>48</v>
-      </c>
-      <c r="F109">
-        <v>0.68313492063492054</v>
-      </c>
-      <c r="G109" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>9</v>
-      </c>
-      <c r="B110">
-        <v>8</v>
-      </c>
-      <c r="C110" t="s">
+    <row r="114" spans="1:7">
+      <c r="A114" t="s">
+        <v>9</v>
+      </c>
+      <c r="B114">
+        <v>8</v>
+      </c>
+      <c r="C114" t="s">
         <v>20</v>
       </c>
-      <c r="D110" t="s">
-        <v>41</v>
-      </c>
-      <c r="E110" t="s">
-        <v>46</v>
-      </c>
-      <c r="F110">
-        <v>0.96621067031463748</v>
-      </c>
-      <c r="G110" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>9</v>
-      </c>
-      <c r="B111">
-        <v>8</v>
-      </c>
-      <c r="C111" t="s">
+      <c r="D114" t="s">
+        <v>43</v>
+      </c>
+      <c r="E114" t="s">
+        <v>50</v>
+      </c>
+      <c r="F114">
+        <v>0.6699999999999999</v>
+      </c>
+      <c r="G114" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115" t="s">
+        <v>9</v>
+      </c>
+      <c r="B115">
+        <v>8</v>
+      </c>
+      <c r="C115" t="s">
         <v>20</v>
       </c>
-      <c r="D111" t="s">
-        <v>41</v>
-      </c>
-      <c r="E111" t="s">
-        <v>47</v>
-      </c>
-      <c r="F111">
-        <v>0.62666666666666671</v>
-      </c>
-      <c r="G111" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>9</v>
-      </c>
-      <c r="B112">
-        <v>8</v>
-      </c>
-      <c r="C112" t="s">
-        <v>20</v>
-      </c>
-      <c r="D112" t="s">
-        <v>41</v>
-      </c>
-      <c r="E112" t="s">
-        <v>48</v>
-      </c>
-      <c r="F112">
-        <v>0.73833333333333329</v>
-      </c>
-      <c r="G112" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>9</v>
-      </c>
-      <c r="B113">
-        <v>8</v>
-      </c>
-      <c r="C113" t="s">
-        <v>19</v>
-      </c>
-      <c r="D113" t="s">
-        <v>42</v>
-      </c>
-      <c r="E113" t="s">
-        <v>46</v>
-      </c>
-      <c r="F113">
-        <v>0.95570451436388504</v>
-      </c>
-      <c r="G113" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>9</v>
-      </c>
-      <c r="B114">
-        <v>8</v>
-      </c>
-      <c r="C114" t="s">
-        <v>19</v>
-      </c>
-      <c r="D114" t="s">
-        <v>42</v>
-      </c>
-      <c r="E114" t="s">
-        <v>47</v>
-      </c>
-      <c r="F114">
-        <v>0.66999999999999993</v>
-      </c>
-      <c r="G114" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>9</v>
-      </c>
-      <c r="B115">
-        <v>8</v>
-      </c>
-      <c r="C115" t="s">
-        <v>19</v>
-      </c>
       <c r="D115" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E115" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F115">
-        <v>0.67154761904761906</v>
+        <v>0.6715476190476191</v>
       </c>
       <c r="G115" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
       <c r="A116" t="s">
         <v>9</v>
       </c>
@@ -3503,22 +3471,22 @@
         <v>8</v>
       </c>
       <c r="C116" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D116" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E116" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F116">
-        <v>0.93707250341997261</v>
+        <v>0.9370725034199726</v>
       </c>
       <c r="G116" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
       <c r="A117" t="s">
         <v>9</v>
       </c>
@@ -3526,22 +3494,22 @@
         <v>8</v>
       </c>
       <c r="C117" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D117" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E117" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F117">
         <v>0.04</v>
       </c>
       <c r="G117" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
       <c r="A118" t="s">
         <v>9</v>
       </c>
@@ -3549,22 +3517,22 @@
         <v>8</v>
       </c>
       <c r="C118" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D118" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E118" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F118">
         <v>0.15</v>
       </c>
       <c r="G118" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
       <c r="A119" t="s">
         <v>9</v>
       </c>
@@ -3572,22 +3540,22 @@
         <v>8</v>
       </c>
       <c r="C119" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D119" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E119" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F119">
-        <v>0.93590971272229828</v>
+        <v>0.9359097127222983</v>
       </c>
       <c r="G119" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
       <c r="A120" t="s">
         <v>9</v>
       </c>
@@ -3595,22 +3563,22 @@
         <v>8</v>
       </c>
       <c r="C120" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D120" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E120" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F120">
         <v>0</v>
       </c>
       <c r="G120" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
       <c r="A121" t="s">
         <v>9</v>
       </c>
@@ -3618,157 +3586,295 @@
         <v>8</v>
       </c>
       <c r="C121" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D121" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E121" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F121">
         <v>0</v>
       </c>
       <c r="G121" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
       <c r="A122" t="s">
         <v>9</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B122">
+        <v>8</v>
+      </c>
+      <c r="C122" t="s">
+        <v>25</v>
+      </c>
+      <c r="D122" t="s">
+        <v>45</v>
+      </c>
+      <c r="E122" t="s">
+        <v>49</v>
+      </c>
+      <c r="F122">
+        <v>0.9662106703146375</v>
+      </c>
+      <c r="G122" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
+      <c r="A123" t="s">
+        <v>9</v>
+      </c>
+      <c r="B123">
+        <v>8</v>
+      </c>
+      <c r="C123" t="s">
+        <v>25</v>
+      </c>
+      <c r="D123" t="s">
+        <v>45</v>
+      </c>
+      <c r="E123" t="s">
+        <v>50</v>
+      </c>
+      <c r="F123">
+        <v>0.7699999999999999</v>
+      </c>
+      <c r="G123" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="A124" t="s">
+        <v>9</v>
+      </c>
+      <c r="B124">
+        <v>8</v>
+      </c>
+      <c r="C124" t="s">
+        <v>25</v>
+      </c>
+      <c r="D124" t="s">
+        <v>45</v>
+      </c>
+      <c r="E124" t="s">
+        <v>51</v>
+      </c>
+      <c r="F124">
+        <v>0.7482142857142857</v>
+      </c>
+      <c r="G124" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
+      <c r="A125" t="s">
+        <v>9</v>
+      </c>
+      <c r="B125">
+        <v>8</v>
+      </c>
+      <c r="C125" t="s">
+        <v>23</v>
+      </c>
+      <c r="D125" t="s">
+        <v>46</v>
+      </c>
+      <c r="E125" t="s">
+        <v>49</v>
+      </c>
+      <c r="F125">
+        <v>0.9615458276333788</v>
+      </c>
+      <c r="G125" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7">
+      <c r="A126" t="s">
+        <v>9</v>
+      </c>
+      <c r="B126">
+        <v>8</v>
+      </c>
+      <c r="C126" t="s">
+        <v>23</v>
+      </c>
+      <c r="D126" t="s">
+        <v>46</v>
+      </c>
+      <c r="E126" t="s">
+        <v>50</v>
+      </c>
+      <c r="F126">
+        <v>0.8766666666666666</v>
+      </c>
+      <c r="G126" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7">
+      <c r="A127" t="s">
+        <v>9</v>
+      </c>
+      <c r="B127">
+        <v>8</v>
+      </c>
+      <c r="C127" t="s">
+        <v>23</v>
+      </c>
+      <c r="D127" t="s">
+        <v>46</v>
+      </c>
+      <c r="E127" t="s">
+        <v>51</v>
+      </c>
+      <c r="F127">
+        <v>0.6831349206349205</v>
+      </c>
+      <c r="G127" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7">
+      <c r="A128" t="s">
         <v>10</v>
       </c>
-      <c r="C122" t="s">
-        <v>24</v>
-      </c>
-      <c r="D122" t="s">
-        <v>44</v>
-      </c>
-      <c r="E122" t="s">
-        <v>46</v>
-      </c>
-      <c r="F122">
-        <v>0.96621067031463748</v>
-      </c>
-      <c r="G122" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>9</v>
-      </c>
-      <c r="B123" t="s">
+      <c r="B128" t="s">
+        <v>11</v>
+      </c>
+      <c r="C128" t="s">
+        <v>18</v>
+      </c>
+      <c r="D128" t="s">
+        <v>47</v>
+      </c>
+      <c r="E128" t="s">
+        <v>49</v>
+      </c>
+      <c r="F128">
+        <v>0.9580711354309166</v>
+      </c>
+      <c r="G128" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7">
+      <c r="A129" t="s">
         <v>10</v>
       </c>
-      <c r="C123" t="s">
-        <v>24</v>
-      </c>
-      <c r="D123" t="s">
-        <v>44</v>
-      </c>
-      <c r="E123" t="s">
+      <c r="B129" t="s">
+        <v>11</v>
+      </c>
+      <c r="C129" t="s">
+        <v>18</v>
+      </c>
+      <c r="D129" t="s">
         <v>47</v>
       </c>
-      <c r="F123">
-        <v>0.76999999999999991</v>
-      </c>
-      <c r="G123" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>9</v>
-      </c>
-      <c r="B124" t="s">
+      <c r="E129" t="s">
+        <v>50</v>
+      </c>
+      <c r="F129">
+        <v>0.6266666666666666</v>
+      </c>
+      <c r="G129" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7">
+      <c r="A130" t="s">
         <v>10</v>
       </c>
-      <c r="C124" t="s">
-        <v>24</v>
-      </c>
-      <c r="D124" t="s">
-        <v>44</v>
-      </c>
-      <c r="E124" t="s">
+      <c r="B130" t="s">
+        <v>11</v>
+      </c>
+      <c r="C130" t="s">
+        <v>18</v>
+      </c>
+      <c r="D130" t="s">
+        <v>47</v>
+      </c>
+      <c r="E130" t="s">
+        <v>51</v>
+      </c>
+      <c r="F130">
+        <v>0.7266666666666667</v>
+      </c>
+      <c r="G130" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7">
+      <c r="A131" t="s">
+        <v>10</v>
+      </c>
+      <c r="B131" t="s">
+        <v>11</v>
+      </c>
+      <c r="C131" t="s">
+        <v>16</v>
+      </c>
+      <c r="D131" t="s">
         <v>48</v>
       </c>
-      <c r="F124">
-        <v>0.74821428571428572</v>
-      </c>
-      <c r="G124" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>9</v>
-      </c>
-      <c r="B125" t="s">
+      <c r="E131" t="s">
+        <v>49</v>
+      </c>
+      <c r="F131">
+        <v>0.9603967168262653</v>
+      </c>
+      <c r="G131" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7">
+      <c r="A132" t="s">
         <v>10</v>
       </c>
-      <c r="C125" t="s">
-        <v>22</v>
-      </c>
-      <c r="D125" t="s">
-        <v>45</v>
-      </c>
-      <c r="E125" t="s">
-        <v>46</v>
-      </c>
-      <c r="F125">
-        <v>0.96154582763337881</v>
-      </c>
-      <c r="G125" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>9</v>
-      </c>
-      <c r="B126" t="s">
+      <c r="B132" t="s">
+        <v>11</v>
+      </c>
+      <c r="C132" t="s">
+        <v>16</v>
+      </c>
+      <c r="D132" t="s">
+        <v>48</v>
+      </c>
+      <c r="E132" t="s">
+        <v>50</v>
+      </c>
+      <c r="F132">
+        <v>0.7766666666666666</v>
+      </c>
+      <c r="G132" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7">
+      <c r="A133" t="s">
         <v>10</v>
       </c>
-      <c r="C126" t="s">
-        <v>22</v>
-      </c>
-      <c r="D126" t="s">
-        <v>45</v>
-      </c>
-      <c r="E126" t="s">
-        <v>47</v>
-      </c>
-      <c r="F126">
-        <v>0.87666666666666659</v>
-      </c>
-      <c r="G126" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>9</v>
-      </c>
-      <c r="B127" t="s">
-        <v>10</v>
-      </c>
-      <c r="C127" t="s">
-        <v>22</v>
-      </c>
-      <c r="D127" t="s">
-        <v>45</v>
-      </c>
-      <c r="E127" t="s">
+      <c r="B133" t="s">
+        <v>11</v>
+      </c>
+      <c r="C133" t="s">
+        <v>16</v>
+      </c>
+      <c r="D133" t="s">
         <v>48</v>
       </c>
-      <c r="F127">
-        <v>0.68313492063492054</v>
-      </c>
-      <c r="G127" t="s">
-        <v>106</v>
+      <c r="E133" t="s">
+        <v>51</v>
+      </c>
+      <c r="F133">
+        <v>0.6861507936507937</v>
+      </c>
+      <c r="G133" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gráficos todos os classificadores
</commit_message>
<xml_diff>
--- a/model_results/all_models_results.xlsx
+++ b/model_results/all_models_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lhsal\Documents\GitHub\projeto_SIN5007_rec_padroes\model_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA99F8A9-ADEA-42CF-B85E-1143B545BBED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AE9DB6-8CC7-428A-94E4-AB91A4524B35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="157">
   <si>
     <t>Algoritmo</t>
   </si>
@@ -479,18 +479,6 @@
   </si>
   <si>
     <t>[0.417, 0.248, 0.585]</t>
-  </si>
-  <si>
-    <t>Branch and Bound - Sem Normalização - Desbalanceado</t>
-  </si>
-  <si>
-    <t>Branch and Bound - Sem Normalização - Balanceado</t>
-  </si>
-  <si>
-    <t>Branch and Bound - Normalizado - Desbalanceado</t>
-  </si>
-  <si>
-    <t>Branch and Bound - Normalizado - Balanceado</t>
   </si>
   <si>
     <t>('rbf', 10, '0.0001')</t>
@@ -587,7 +575,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -909,21 +897,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="G171" sqref="G171:G173"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="C166" sqref="C166"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="57.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.42578125" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -946,7 +934,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -969,7 +957,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -992,7 +980,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1015,7 +1003,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1038,7 +1026,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1061,7 +1049,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1084,7 +1072,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1107,7 +1095,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1130,7 +1118,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1153,7 +1141,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1176,7 +1164,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1199,7 +1187,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1222,7 +1210,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1245,7 +1233,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1268,7 +1256,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1291,7 +1279,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1314,7 +1302,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1337,7 +1325,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1360,7 +1348,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1383,7 +1371,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1406,7 +1394,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1429,7 +1417,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1452,7 +1440,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1475,7 +1463,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -1498,7 +1486,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1521,7 +1509,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1544,7 +1532,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1567,7 +1555,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1590,7 +1578,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -1613,7 +1601,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1636,7 +1624,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1659,7 +1647,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1682,7 +1670,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -1705,7 +1693,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -1728,7 +1716,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -1751,7 +1739,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -1774,7 +1762,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -1797,7 +1785,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -1820,7 +1808,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -1843,7 +1831,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -1866,7 +1854,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -1889,7 +1877,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -1912,7 +1900,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -1935,7 +1923,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -1958,7 +1946,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -1981,7 +1969,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -2004,7 +1992,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -2027,7 +2015,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -2050,7 +2038,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -2073,7 +2061,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -2096,7 +2084,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -2119,7 +2107,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -2142,7 +2130,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -2165,7 +2153,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -2188,7 +2176,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -2211,7 +2199,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>10</v>
       </c>
@@ -2234,7 +2222,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>10</v>
       </c>
@@ -2257,7 +2245,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>10</v>
       </c>
@@ -2280,7 +2268,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -2303,7 +2291,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>10</v>
       </c>
@@ -2326,7 +2314,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -2349,7 +2337,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>10</v>
       </c>
@@ -2372,7 +2360,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>10</v>
       </c>
@@ -2395,7 +2383,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>10</v>
       </c>
@@ -2418,7 +2406,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>10</v>
       </c>
@@ -2441,7 +2429,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>10</v>
       </c>
@@ -2464,7 +2452,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -2487,7 +2475,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>10</v>
       </c>
@@ -2510,7 +2498,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>10</v>
       </c>
@@ -2533,7 +2521,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>10</v>
       </c>
@@ -2556,7 +2544,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>10</v>
       </c>
@@ -2579,7 +2567,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>10</v>
       </c>
@@ -2602,7 +2590,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -2625,7 +2613,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>8</v>
       </c>
@@ -2648,7 +2636,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>8</v>
       </c>
@@ -2671,7 +2659,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>8</v>
       </c>
@@ -2694,7 +2682,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>8</v>
       </c>
@@ -2717,7 +2705,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>8</v>
       </c>
@@ -2740,7 +2728,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>8</v>
       </c>
@@ -2763,7 +2751,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>8</v>
       </c>
@@ -2786,7 +2774,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>8</v>
       </c>
@@ -2809,7 +2797,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>8</v>
       </c>
@@ -2832,7 +2820,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>8</v>
       </c>
@@ -2855,7 +2843,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>8</v>
       </c>
@@ -2878,7 +2866,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>8</v>
       </c>
@@ -2901,7 +2889,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>8</v>
       </c>
@@ -2924,7 +2912,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>8</v>
       </c>
@@ -2947,7 +2935,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>8</v>
       </c>
@@ -2970,7 +2958,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>8</v>
       </c>
@@ -2993,7 +2981,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>8</v>
       </c>
@@ -3016,7 +3004,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>8</v>
       </c>
@@ -3039,7 +3027,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>8</v>
       </c>
@@ -3062,7 +3050,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>8</v>
       </c>
@@ -3085,7 +3073,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>8</v>
       </c>
@@ -3108,7 +3096,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>8</v>
       </c>
@@ -3131,7 +3119,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>8</v>
       </c>
@@ -3154,7 +3142,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>8</v>
       </c>
@@ -3177,7 +3165,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>8</v>
       </c>
@@ -3200,7 +3188,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>8</v>
       </c>
@@ -3223,7 +3211,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>8</v>
       </c>
@@ -3246,7 +3234,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>8</v>
       </c>
@@ -3269,7 +3257,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>8</v>
       </c>
@@ -3292,7 +3280,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>8</v>
       </c>
@@ -3315,7 +3303,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>8</v>
       </c>
@@ -3338,7 +3326,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>8</v>
       </c>
@@ -3361,7 +3349,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>8</v>
       </c>
@@ -3384,7 +3372,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>8</v>
       </c>
@@ -3407,7 +3395,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>8</v>
       </c>
@@ -3430,7 +3418,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>8</v>
       </c>
@@ -3453,7 +3441,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>8</v>
       </c>
@@ -3476,7 +3464,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>8</v>
       </c>
@@ -3499,7 +3487,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>8</v>
       </c>
@@ -3522,7 +3510,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>8</v>
       </c>
@@ -3545,7 +3533,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>8</v>
       </c>
@@ -3568,7 +3556,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>9</v>
       </c>
@@ -3591,7 +3579,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>9</v>
       </c>
@@ -3614,7 +3602,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>9</v>
       </c>
@@ -3637,7 +3625,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>9</v>
       </c>
@@ -3660,7 +3648,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>9</v>
       </c>
@@ -3683,7 +3671,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>9</v>
       </c>
@@ -3706,7 +3694,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>9</v>
       </c>
@@ -3729,7 +3717,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>9</v>
       </c>
@@ -3752,7 +3740,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>9</v>
       </c>
@@ -3775,7 +3763,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>9</v>
       </c>
@@ -3798,7 +3786,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>9</v>
       </c>
@@ -3821,7 +3809,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>9</v>
       </c>
@@ -3844,7 +3832,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>9</v>
       </c>
@@ -3867,7 +3855,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>9</v>
       </c>
@@ -3890,7 +3878,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>9</v>
       </c>
@@ -3913,7 +3901,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>9</v>
       </c>
@@ -3936,7 +3924,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>9</v>
       </c>
@@ -3959,7 +3947,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>9</v>
       </c>
@@ -3982,7 +3970,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>9</v>
       </c>
@@ -4005,7 +3993,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>9</v>
       </c>
@@ -4028,7 +4016,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>9</v>
       </c>
@@ -4051,7 +4039,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>9</v>
       </c>
@@ -4074,7 +4062,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>9</v>
       </c>
@@ -4097,7 +4085,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>9</v>
       </c>
@@ -4120,7 +4108,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>9</v>
       </c>
@@ -4143,7 +4131,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>9</v>
       </c>
@@ -4166,7 +4154,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>9</v>
       </c>
@@ -4189,7 +4177,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>9</v>
       </c>
@@ -4212,7 +4200,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>9</v>
       </c>
@@ -4235,7 +4223,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>9</v>
       </c>
@@ -4258,7 +4246,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>9</v>
       </c>
@@ -4281,7 +4269,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>9</v>
       </c>
@@ -4304,7 +4292,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>9</v>
       </c>
@@ -4327,7 +4315,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>9</v>
       </c>
@@ -4350,7 +4338,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>9</v>
       </c>
@@ -4373,7 +4361,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>9</v>
       </c>
@@ -4396,7 +4384,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>9</v>
       </c>
@@ -4419,7 +4407,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>9</v>
       </c>
@@ -4442,7 +4430,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>9</v>
       </c>
@@ -4465,7 +4453,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>9</v>
       </c>
@@ -4488,7 +4476,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>9</v>
       </c>
@@ -4511,7 +4499,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>9</v>
       </c>
@@ -4534,7 +4522,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>7</v>
       </c>
@@ -4542,7 +4530,7 @@
         <v>7</v>
       </c>
       <c r="C158" t="s">
-        <v>154</v>
+        <v>24</v>
       </c>
       <c r="D158" t="s">
         <v>27</v>
@@ -4557,7 +4545,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>7</v>
       </c>
@@ -4565,7 +4553,7 @@
         <v>7</v>
       </c>
       <c r="C159" t="s">
-        <v>154</v>
+        <v>24</v>
       </c>
       <c r="D159" t="s">
         <v>27</v>
@@ -4580,7 +4568,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>7</v>
       </c>
@@ -4588,7 +4576,7 @@
         <v>7</v>
       </c>
       <c r="C160" t="s">
-        <v>154</v>
+        <v>24</v>
       </c>
       <c r="D160" t="s">
         <v>27</v>
@@ -4600,10 +4588,10 @@
         <v>0.7533333333333333</v>
       </c>
       <c r="G160" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>7</v>
       </c>
@@ -4611,10 +4599,10 @@
         <v>7</v>
       </c>
       <c r="C161" t="s">
-        <v>155</v>
+        <v>25</v>
       </c>
       <c r="D161" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E161" t="s">
         <v>53</v>
@@ -4626,7 +4614,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>7</v>
       </c>
@@ -4634,10 +4622,10 @@
         <v>7</v>
       </c>
       <c r="C162" t="s">
-        <v>155</v>
+        <v>25</v>
       </c>
       <c r="D162" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E162" t="s">
         <v>54</v>
@@ -4649,7 +4637,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>7</v>
       </c>
@@ -4657,10 +4645,10 @@
         <v>7</v>
       </c>
       <c r="C163" t="s">
-        <v>155</v>
+        <v>25</v>
       </c>
       <c r="D163" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E163" t="s">
         <v>55</v>
@@ -4669,10 +4657,10 @@
         <v>0.7533333333333333</v>
       </c>
       <c r="G163" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>7</v>
       </c>
@@ -4680,7 +4668,7 @@
         <v>7</v>
       </c>
       <c r="C164" t="s">
-        <v>152</v>
+        <v>22</v>
       </c>
       <c r="D164" t="s">
         <v>27</v>
@@ -4695,7 +4683,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>7</v>
       </c>
@@ -4703,7 +4691,7 @@
         <v>7</v>
       </c>
       <c r="C165" t="s">
-        <v>152</v>
+        <v>22</v>
       </c>
       <c r="D165" t="s">
         <v>27</v>
@@ -4718,7 +4706,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>7</v>
       </c>
@@ -4726,7 +4714,7 @@
         <v>7</v>
       </c>
       <c r="C166" t="s">
-        <v>152</v>
+        <v>22</v>
       </c>
       <c r="D166" t="s">
         <v>27</v>
@@ -4738,10 +4726,10 @@
         <v>0.7533333333333333</v>
       </c>
       <c r="G166" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>7</v>
       </c>
@@ -4749,7 +4737,7 @@
         <v>7</v>
       </c>
       <c r="C167" t="s">
-        <v>153</v>
+        <v>23</v>
       </c>
       <c r="D167" t="s">
         <v>27</v>
@@ -4761,10 +4749,10 @@
         <v>0.94060191518467851</v>
       </c>
       <c r="G167" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.35">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>7</v>
       </c>
@@ -4772,7 +4760,7 @@
         <v>7</v>
       </c>
       <c r="C168" t="s">
-        <v>153</v>
+        <v>23</v>
       </c>
       <c r="D168" t="s">
         <v>27</v>
@@ -4784,10 +4772,10 @@
         <v>0.47333333333333327</v>
       </c>
       <c r="G168" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.35">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>7</v>
       </c>
@@ -4795,7 +4783,7 @@
         <v>7</v>
       </c>
       <c r="C169" t="s">
-        <v>153</v>
+        <v>23</v>
       </c>
       <c r="D169" t="s">
         <v>27</v>
@@ -4807,7 +4795,7 @@
         <v>0.72098039215686271</v>
       </c>
       <c r="G169" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adicionado qtd de caracteristicas por condicao nos graficos de resultados
</commit_message>
<xml_diff>
--- a/model_results/all_models_results.xlsx
+++ b/model_results/all_models_results.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lhsal\Documents\GitHub\projeto_SIN5007_rec_padroes\model_results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Mestrado\projeto_SIN5007_rec_padroes\model_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AE9DB6-8CC7-428A-94E4-AB91A4524B35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85DF0C5-6925-49FB-B28B-1D20B015F0DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$157</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$169</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -61,48 +61,6 @@
     <t>9</t>
   </si>
   <si>
-    <t>Dataset Completo Balanceado - Nao Normalizado</t>
-  </si>
-  <si>
-    <t>Dataset Completo Balanceado - Normalizado</t>
-  </si>
-  <si>
-    <t>Dataset Completo Desbalanceado - Nao Normalizado</t>
-  </si>
-  <si>
-    <t>Dataset Completo Desbalanceado - Normalizado</t>
-  </si>
-  <si>
-    <t>PCA Balanceado</t>
-  </si>
-  <si>
-    <t>PCA Desbalanceado</t>
-  </si>
-  <si>
-    <t>ReliefF Balanceado - Nao Normalizado</t>
-  </si>
-  <si>
-    <t>ReliefF Balanceado - Normalizado</t>
-  </si>
-  <si>
-    <t>ReliefF Desbalanceado - Nao Normalizado</t>
-  </si>
-  <si>
-    <t>ReliefF Desbalanceado - Normalizado</t>
-  </si>
-  <si>
-    <t>Branch and Bound Desbalanceado - Nao Normalizado</t>
-  </si>
-  <si>
-    <t>Branch and Bound Balanceado - Nao Normalizado</t>
-  </si>
-  <si>
-    <t>Branch and Bound Desbalanceado - Normalizado</t>
-  </si>
-  <si>
-    <t>Branch and Bound Balanceado - Normalizado</t>
-  </si>
-  <si>
     <t>('rbf', 100, '0.0001')</t>
   </si>
   <si>
@@ -494,6 +452,48 @@
   </si>
   <si>
     <t>[0.721, 0.481, 0.961]</t>
+  </si>
+  <si>
+    <t>Dataset Completo Balanceado - Nao Normalizado (35)</t>
+  </si>
+  <si>
+    <t>Branch and Bound Balanceado - Nao Normalizado (6)</t>
+  </si>
+  <si>
+    <t>Branch and Bound Balanceado - Normalizado (6)</t>
+  </si>
+  <si>
+    <t>Branch and Bound Desbalanceado - Nao Normalizado (6)</t>
+  </si>
+  <si>
+    <t>Branch and Bound Desbalanceado - Normalizado (6)</t>
+  </si>
+  <si>
+    <t>Dataset Completo Balanceado - Normalizado (35)</t>
+  </si>
+  <si>
+    <t>Dataset Completo Desbalanceado - Nao Normalizado (35)</t>
+  </si>
+  <si>
+    <t>Dataset Completo Desbalanceado - Normalizado (35)</t>
+  </si>
+  <si>
+    <t>PCA Balanceado (12)</t>
+  </si>
+  <si>
+    <t>PCA Desbalanceado (12)</t>
+  </si>
+  <si>
+    <t>ReliefF Balanceado - Nao Normalizado (10)</t>
+  </si>
+  <si>
+    <t>ReliefF Balanceado - Normalizado (10)</t>
+  </si>
+  <si>
+    <t>ReliefF Desbalanceado - Nao Normalizado (10)</t>
+  </si>
+  <si>
+    <t>ReliefF Desbalanceado - Normalizado (10)</t>
   </si>
 </sst>
 </file>
@@ -575,7 +575,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -897,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="C166" sqref="C166"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,19 +942,19 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F2">
         <v>0.96270861833105337</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -965,19 +965,19 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F3">
         <v>0.87666666666666659</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -988,19 +988,19 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F4">
         <v>0.69007936507936507</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1011,19 +1011,19 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>148</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F5">
         <v>0.95919288645690826</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1034,19 +1034,19 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>148</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F6">
         <v>0.91000000000000014</v>
       </c>
       <c r="G6" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1057,19 +1057,19 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>148</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F7">
         <v>0.67301587301587307</v>
       </c>
       <c r="G7" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1080,19 +1080,19 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F8">
         <v>0.96038303693570448</v>
       </c>
       <c r="G8" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1103,19 +1103,19 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F9">
         <v>0.86</v>
       </c>
       <c r="G9" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1126,19 +1126,19 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F10">
         <v>0.677579365079365</v>
       </c>
       <c r="G10" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1149,19 +1149,19 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>150</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F11">
         <v>0.96270861833105337</v>
       </c>
       <c r="G11" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1172,19 +1172,19 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>150</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F12">
         <v>0.87666666666666659</v>
       </c>
       <c r="G12" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1195,19 +1195,19 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>150</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F13">
         <v>0.69007936507936507</v>
       </c>
       <c r="G13" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1218,19 +1218,19 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>151</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F14">
         <v>0.9580574555403556</v>
       </c>
       <c r="G14" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1241,19 +1241,19 @@
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>151</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F15">
         <v>0.71666666666666656</v>
       </c>
       <c r="G15" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1264,19 +1264,19 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>151</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F16">
         <v>0.71380952380952378</v>
       </c>
       <c r="G16" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1287,19 +1287,19 @@
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>152</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F17">
         <v>0.96389876880984937</v>
       </c>
       <c r="G17" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1310,19 +1310,19 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>152</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F18">
         <v>0.6399999999999999</v>
       </c>
       <c r="G18" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1333,19 +1333,19 @@
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>152</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F19">
         <v>0.79952380952380953</v>
       </c>
       <c r="G19" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1356,19 +1356,19 @@
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F20">
         <v>0.96270861833105337</v>
       </c>
       <c r="G20" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1379,19 +1379,19 @@
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F21">
         <v>0.87666666666666659</v>
       </c>
       <c r="G21" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1402,19 +1402,19 @@
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E22" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F22">
         <v>0.69007936507936507</v>
       </c>
       <c r="G22" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1425,19 +1425,19 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>154</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E23" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F23">
         <v>0.9638714090287277</v>
       </c>
       <c r="G23" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1448,19 +1448,19 @@
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>154</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E24" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F24">
         <v>0.87666666666666659</v>
       </c>
       <c r="G24" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1471,19 +1471,19 @@
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>154</v>
       </c>
       <c r="D25" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E25" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F25">
         <v>0.69722222222222219</v>
       </c>
       <c r="G25" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1494,19 +1494,19 @@
         <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>155</v>
       </c>
       <c r="D26" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E26" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F26">
         <v>0.96154582763337881</v>
       </c>
       <c r="G26" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1517,19 +1517,19 @@
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>20</v>
+        <v>155</v>
       </c>
       <c r="D27" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E27" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F27">
         <v>0.87666666666666659</v>
       </c>
       <c r="G27" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1540,19 +1540,19 @@
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>20</v>
+        <v>155</v>
       </c>
       <c r="D28" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E28" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F28">
         <v>0.68313492063492054</v>
       </c>
       <c r="G28" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1563,19 +1563,19 @@
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>21</v>
+        <v>156</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E29" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F29">
         <v>0.96154582763337904</v>
       </c>
       <c r="G29" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1586,19 +1586,19 @@
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>21</v>
+        <v>156</v>
       </c>
       <c r="D30" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E30" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F30">
         <v>0.65999999999999992</v>
       </c>
       <c r="G30" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1609,19 +1609,19 @@
         <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>21</v>
+        <v>156</v>
       </c>
       <c r="D31" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E31" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F31">
         <v>0.73666666666666658</v>
       </c>
       <c r="G31" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1632,19 +1632,19 @@
         <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
       <c r="D32" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E32" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F32">
         <v>0.96154582763337881</v>
       </c>
       <c r="G32" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1655,19 +1655,19 @@
         <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
       <c r="D33" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E33" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F33">
         <v>0.87666666666666659</v>
       </c>
       <c r="G33" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1678,19 +1678,19 @@
         <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
       <c r="D34" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E34" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F34">
         <v>0.68313492063492054</v>
       </c>
       <c r="G34" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1701,19 +1701,19 @@
         <v>9</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>143</v>
       </c>
       <c r="D35" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E35" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F35">
         <v>0.96737346101231181</v>
       </c>
       <c r="G35" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1724,19 +1724,19 @@
         <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>12</v>
+        <v>143</v>
       </c>
       <c r="D36" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E36" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F36">
         <v>0.86</v>
       </c>
       <c r="G36" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1747,19 +1747,19 @@
         <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
+        <v>143</v>
       </c>
       <c r="D37" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E37" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F37">
         <v>0.72757936507936516</v>
       </c>
       <c r="G37" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1770,19 +1770,19 @@
         <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>15</v>
+        <v>150</v>
       </c>
       <c r="D38" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E38" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F38">
         <v>0.96154582763337881</v>
       </c>
       <c r="G38" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1793,19 +1793,19 @@
         <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>15</v>
+        <v>150</v>
       </c>
       <c r="D39" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E39" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F39">
         <v>0.87666666666666659</v>
       </c>
       <c r="G39" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1816,19 +1816,19 @@
         <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>15</v>
+        <v>150</v>
       </c>
       <c r="D40" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E40" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F40">
         <v>0.68313492063492054</v>
       </c>
       <c r="G40" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1839,19 +1839,19 @@
         <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>13</v>
+        <v>148</v>
       </c>
       <c r="D41" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E41" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F41">
         <v>0.96737346101231181</v>
       </c>
       <c r="G41" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1862,19 +1862,19 @@
         <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>13</v>
+        <v>148</v>
       </c>
       <c r="D42" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E42" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F42">
         <v>0.86</v>
       </c>
       <c r="G42" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1885,19 +1885,19 @@
         <v>9</v>
       </c>
       <c r="C43" t="s">
-        <v>13</v>
+        <v>148</v>
       </c>
       <c r="D43" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E43" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F43">
         <v>0.72757936507936516</v>
       </c>
       <c r="G43" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1908,19 +1908,19 @@
         <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>17</v>
+        <v>152</v>
       </c>
       <c r="D44" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="E44" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F44">
         <v>0.95923392612859093</v>
       </c>
       <c r="G44" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1931,19 +1931,19 @@
         <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>17</v>
+        <v>152</v>
       </c>
       <c r="D45" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="E45" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F45">
         <v>0.60333333333333328</v>
       </c>
       <c r="G45" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1954,19 +1954,19 @@
         <v>9</v>
       </c>
       <c r="C46" t="s">
-        <v>17</v>
+        <v>152</v>
       </c>
       <c r="D46" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="E46" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F46">
         <v>0.77523809523809528</v>
       </c>
       <c r="G46" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -1977,19 +1977,19 @@
         <v>9</v>
       </c>
       <c r="C47" t="s">
-        <v>16</v>
+        <v>151</v>
       </c>
       <c r="D47" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="E47" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F47">
         <v>0.94638850889192871</v>
       </c>
       <c r="G47" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2000,19 +2000,19 @@
         <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>16</v>
+        <v>151</v>
       </c>
       <c r="D48" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="E48" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F48">
         <v>0.7433333333333334</v>
       </c>
       <c r="G48" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2023,19 +2023,19 @@
         <v>9</v>
       </c>
       <c r="C49" t="s">
-        <v>16</v>
+        <v>151</v>
       </c>
       <c r="D49" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="E49" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F49">
         <v>0.60160173160173158</v>
       </c>
       <c r="G49" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2046,19 +2046,19 @@
         <v>9</v>
       </c>
       <c r="C50" t="s">
-        <v>20</v>
+        <v>155</v>
       </c>
       <c r="D50" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="E50" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F50">
         <v>0.96504787961696292</v>
       </c>
       <c r="G50" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2069,19 +2069,19 @@
         <v>9</v>
       </c>
       <c r="C51" t="s">
-        <v>20</v>
+        <v>155</v>
       </c>
       <c r="D51" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="E51" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F51">
         <v>0.77333333333333321</v>
       </c>
       <c r="G51" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2092,19 +2092,19 @@
         <v>9</v>
       </c>
       <c r="C52" t="s">
-        <v>20</v>
+        <v>155</v>
       </c>
       <c r="D52" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="E52" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F52">
         <v>0.73345238095238086</v>
       </c>
       <c r="G52" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2115,19 +2115,19 @@
         <v>9</v>
       </c>
       <c r="C53" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="D53" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E53" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F53">
         <v>0.96388508891928859</v>
       </c>
       <c r="G53" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2138,19 +2138,19 @@
         <v>9</v>
       </c>
       <c r="C54" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="D54" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E54" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F54">
         <v>0.84000000000000008</v>
       </c>
       <c r="G54" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2161,19 +2161,19 @@
         <v>9</v>
       </c>
       <c r="C55" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="D55" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E55" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F55">
         <v>0.70777777777777773</v>
       </c>
       <c r="G55" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2184,19 +2184,19 @@
         <v>9</v>
       </c>
       <c r="C56" t="s">
-        <v>21</v>
+        <v>156</v>
       </c>
       <c r="D56" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="E56" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F56">
         <v>0.96388508891928859</v>
       </c>
       <c r="G56" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2207,19 +2207,19 @@
         <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>21</v>
+        <v>156</v>
       </c>
       <c r="D57" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="E57" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F57">
         <v>0.73666666666666658</v>
       </c>
       <c r="G57" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2230,19 +2230,19 @@
         <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>21</v>
+        <v>156</v>
       </c>
       <c r="D58" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="E58" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F58">
         <v>0.74964285714285706</v>
       </c>
       <c r="G58" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2253,19 +2253,19 @@
         <v>9</v>
       </c>
       <c r="C59" t="s">
-        <v>19</v>
+        <v>154</v>
       </c>
       <c r="D59" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E59" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F59">
         <v>0.96388508891928859</v>
       </c>
       <c r="G59" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2276,19 +2276,19 @@
         <v>9</v>
       </c>
       <c r="C60" t="s">
-        <v>19</v>
+        <v>154</v>
       </c>
       <c r="D60" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E60" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F60">
         <v>0.84000000000000008</v>
       </c>
       <c r="G60" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -2299,19 +2299,19 @@
         <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>19</v>
+        <v>154</v>
       </c>
       <c r="D61" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E61" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F61">
         <v>0.70777777777777773</v>
       </c>
       <c r="G61" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2322,19 +2322,19 @@
         <v>9</v>
       </c>
       <c r="C62" t="s">
-        <v>22</v>
+        <v>146</v>
       </c>
       <c r="D62" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E62" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F62">
         <v>0.95339261285909715</v>
       </c>
       <c r="G62" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2345,19 +2345,19 @@
         <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>22</v>
+        <v>146</v>
       </c>
       <c r="D63" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E63" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F63">
         <v>0.45333333333333331</v>
       </c>
       <c r="G63" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2368,19 +2368,19 @@
         <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>22</v>
+        <v>146</v>
       </c>
       <c r="D64" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E64" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F64">
         <v>0.7533333333333333</v>
       </c>
       <c r="G64" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2391,19 +2391,19 @@
         <v>9</v>
       </c>
       <c r="C65" t="s">
-        <v>23</v>
+        <v>144</v>
       </c>
       <c r="D65" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E65" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F65">
         <v>0.95339261285909715</v>
       </c>
       <c r="G65" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2414,19 +2414,19 @@
         <v>9</v>
       </c>
       <c r="C66" t="s">
-        <v>23</v>
+        <v>144</v>
       </c>
       <c r="D66" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E66" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F66">
         <v>0.45333333333333331</v>
       </c>
       <c r="G66" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -2437,19 +2437,19 @@
         <v>9</v>
       </c>
       <c r="C67" t="s">
-        <v>23</v>
+        <v>144</v>
       </c>
       <c r="D67" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E67" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F67">
         <v>0.7533333333333333</v>
       </c>
       <c r="G67" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -2460,19 +2460,19 @@
         <v>11</v>
       </c>
       <c r="C68" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="D68" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E68" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F68">
         <v>0.95339261285909715</v>
       </c>
       <c r="G68" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -2483,19 +2483,19 @@
         <v>11</v>
       </c>
       <c r="C69" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="D69" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E69" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F69">
         <v>0.45333333333333331</v>
       </c>
       <c r="G69" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -2506,19 +2506,19 @@
         <v>11</v>
       </c>
       <c r="C70" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="D70" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E70" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F70">
         <v>0.7533333333333333</v>
       </c>
       <c r="G70" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -2529,19 +2529,19 @@
         <v>11</v>
       </c>
       <c r="C71" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="D71" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E71" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F71">
         <v>0.95339261285909715</v>
       </c>
       <c r="G71" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2552,19 +2552,19 @@
         <v>11</v>
       </c>
       <c r="C72" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="D72" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E72" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F72">
         <v>0.45333333333333331</v>
       </c>
       <c r="G72" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2575,19 +2575,19 @@
         <v>11</v>
       </c>
       <c r="C73" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="D73" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E73" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F73">
         <v>0.7533333333333333</v>
       </c>
       <c r="G73" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2598,19 +2598,19 @@
         <v>6</v>
       </c>
       <c r="C74" t="s">
-        <v>12</v>
+        <v>143</v>
       </c>
       <c r="D74">
         <v>0.8</v>
       </c>
       <c r="E74" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F74">
         <v>0.93932968536251715</v>
       </c>
       <c r="G74" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2621,19 +2621,19 @@
         <v>6</v>
       </c>
       <c r="C75" t="s">
-        <v>12</v>
+        <v>143</v>
       </c>
       <c r="D75">
         <v>0.8</v>
       </c>
       <c r="E75" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F75">
         <v>0.87666666666666659</v>
       </c>
       <c r="G75" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2644,19 +2644,19 @@
         <v>6</v>
       </c>
       <c r="C76" t="s">
-        <v>12</v>
+        <v>143</v>
       </c>
       <c r="D76">
         <v>0.8</v>
       </c>
       <c r="E76" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F76">
         <v>0.54714285714285704</v>
       </c>
       <c r="G76" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2667,19 +2667,19 @@
         <v>6</v>
       </c>
       <c r="C77" t="s">
-        <v>13</v>
+        <v>148</v>
       </c>
       <c r="D77">
         <v>0.2</v>
       </c>
       <c r="E77" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F77">
         <v>0.93584131326949382</v>
       </c>
       <c r="G77" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -2690,19 +2690,19 @@
         <v>6</v>
       </c>
       <c r="C78" t="s">
-        <v>13</v>
+        <v>148</v>
       </c>
       <c r="D78">
         <v>0.2</v>
       </c>
       <c r="E78" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F78">
         <v>0.87666666666666659</v>
       </c>
       <c r="G78" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -2713,19 +2713,19 @@
         <v>6</v>
       </c>
       <c r="C79" t="s">
-        <v>13</v>
+        <v>148</v>
       </c>
       <c r="D79">
         <v>0.2</v>
       </c>
       <c r="E79" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F79">
         <v>0.52769841269841267</v>
       </c>
       <c r="G79" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -2736,19 +2736,19 @@
         <v>6</v>
       </c>
       <c r="C80" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
       <c r="D80">
         <v>0.6</v>
       </c>
       <c r="E80" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F80">
         <v>0.95567715458276337</v>
       </c>
       <c r="G80" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -2759,19 +2759,19 @@
         <v>6</v>
       </c>
       <c r="C81" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
       <c r="D81">
         <v>0.6</v>
       </c>
       <c r="E81" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F81">
         <v>0.71666666666666656</v>
       </c>
       <c r="G81" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -2782,19 +2782,19 @@
         <v>6</v>
       </c>
       <c r="C82" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
       <c r="D82">
         <v>0.6</v>
       </c>
       <c r="E82" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F82">
         <v>0.67539682539682544</v>
       </c>
       <c r="G82" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -2805,19 +2805,19 @@
         <v>6</v>
       </c>
       <c r="C83" t="s">
-        <v>15</v>
+        <v>150</v>
       </c>
       <c r="D83">
         <v>0.9</v>
       </c>
       <c r="E83" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F83">
         <v>0.94753761969904249</v>
       </c>
       <c r="G83" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -2828,19 +2828,19 @@
         <v>6</v>
       </c>
       <c r="C84" t="s">
-        <v>15</v>
+        <v>150</v>
       </c>
       <c r="D84">
         <v>0.9</v>
       </c>
       <c r="E84" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F84">
         <v>0.71666666666666656</v>
       </c>
       <c r="G84" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -2851,19 +2851,19 @@
         <v>6</v>
       </c>
       <c r="C85" t="s">
-        <v>15</v>
+        <v>150</v>
       </c>
       <c r="D85">
         <v>0.9</v>
       </c>
       <c r="E85" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F85">
         <v>0.60444444444444445</v>
       </c>
       <c r="G85" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -2874,19 +2874,19 @@
         <v>6</v>
       </c>
       <c r="C86" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="D86">
         <v>0.1</v>
       </c>
       <c r="E86" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F86">
         <v>0.95689466484268126</v>
       </c>
       <c r="G86" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -2897,19 +2897,19 @@
         <v>6</v>
       </c>
       <c r="C87" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="D87">
         <v>0.1</v>
       </c>
       <c r="E87" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F87">
         <v>0.87666666666666659</v>
       </c>
       <c r="G87" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -2920,19 +2920,19 @@
         <v>6</v>
       </c>
       <c r="C88" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="D88">
         <v>0.1</v>
       </c>
       <c r="E88" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F88">
         <v>0.65230158730158727</v>
       </c>
       <c r="G88" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -2943,19 +2943,19 @@
         <v>6</v>
       </c>
       <c r="C89" t="s">
-        <v>19</v>
+        <v>154</v>
       </c>
       <c r="D89">
         <v>0.2</v>
       </c>
       <c r="E89" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F89">
         <v>0.95689466484268126</v>
       </c>
       <c r="G89" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -2966,19 +2966,19 @@
         <v>6</v>
       </c>
       <c r="C90" t="s">
-        <v>19</v>
+        <v>154</v>
       </c>
       <c r="D90">
         <v>0.2</v>
       </c>
       <c r="E90" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F90">
         <v>0.87666666666666659</v>
       </c>
       <c r="G90" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -2989,19 +2989,19 @@
         <v>6</v>
       </c>
       <c r="C91" t="s">
-        <v>19</v>
+        <v>154</v>
       </c>
       <c r="D91">
         <v>0.2</v>
       </c>
       <c r="E91" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F91">
         <v>0.65230158730158727</v>
       </c>
       <c r="G91" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -3012,19 +3012,19 @@
         <v>6</v>
       </c>
       <c r="C92" t="s">
-        <v>20</v>
+        <v>155</v>
       </c>
       <c r="D92">
         <v>0.4</v>
       </c>
       <c r="E92" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F92">
         <v>0.96272229822161415</v>
       </c>
       <c r="G92" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -3035,19 +3035,19 @@
         <v>6</v>
       </c>
       <c r="C93" t="s">
-        <v>20</v>
+        <v>155</v>
       </c>
       <c r="D93">
         <v>0.4</v>
       </c>
       <c r="E93" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F93">
         <v>0.69666666666666666</v>
       </c>
       <c r="G93" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -3058,19 +3058,19 @@
         <v>6</v>
       </c>
       <c r="C94" t="s">
-        <v>20</v>
+        <v>155</v>
       </c>
       <c r="D94">
         <v>0.4</v>
       </c>
       <c r="E94" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F94">
         <v>0.75380952380952393</v>
       </c>
       <c r="G94" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -3081,19 +3081,19 @@
         <v>6</v>
       </c>
       <c r="C95" t="s">
-        <v>21</v>
+        <v>156</v>
       </c>
       <c r="D95">
         <v>0.8</v>
       </c>
       <c r="E95" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F95">
         <v>0.96272229822161415</v>
       </c>
       <c r="G95" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -3104,19 +3104,19 @@
         <v>6</v>
       </c>
       <c r="C96" t="s">
-        <v>21</v>
+        <v>156</v>
       </c>
       <c r="D96">
         <v>0.8</v>
       </c>
       <c r="E96" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F96">
         <v>0.69666666666666666</v>
       </c>
       <c r="G96" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -3127,19 +3127,19 @@
         <v>6</v>
       </c>
       <c r="C97" t="s">
-        <v>21</v>
+        <v>156</v>
       </c>
       <c r="D97">
         <v>0.8</v>
       </c>
       <c r="E97" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F97">
         <v>0.75380952380952393</v>
       </c>
       <c r="G97" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -3150,19 +3150,19 @@
         <v>6</v>
       </c>
       <c r="C98" t="s">
-        <v>22</v>
+        <v>146</v>
       </c>
       <c r="D98">
         <v>0.5</v>
       </c>
       <c r="E98" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F98">
         <v>0.95339261285909715</v>
       </c>
       <c r="G98" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -3173,19 +3173,19 @@
         <v>6</v>
       </c>
       <c r="C99" t="s">
-        <v>22</v>
+        <v>146</v>
       </c>
       <c r="D99">
         <v>0.5</v>
       </c>
       <c r="E99" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F99">
         <v>0.45333333333333331</v>
       </c>
       <c r="G99" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -3196,19 +3196,19 @@
         <v>6</v>
       </c>
       <c r="C100" t="s">
-        <v>22</v>
+        <v>146</v>
       </c>
       <c r="D100">
         <v>0.5</v>
       </c>
       <c r="E100" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F100">
         <v>0.7533333333333333</v>
       </c>
       <c r="G100" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -3219,19 +3219,19 @@
         <v>6</v>
       </c>
       <c r="C101" t="s">
-        <v>23</v>
+        <v>144</v>
       </c>
       <c r="D101">
         <v>0.4</v>
       </c>
       <c r="E101" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F101">
         <v>0.95339261285909715</v>
       </c>
       <c r="G101" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -3242,19 +3242,19 @@
         <v>6</v>
       </c>
       <c r="C102" t="s">
-        <v>23</v>
+        <v>144</v>
       </c>
       <c r="D102">
         <v>0.4</v>
       </c>
       <c r="E102" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F102">
         <v>0.45333333333333331</v>
       </c>
       <c r="G102" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -3265,19 +3265,19 @@
         <v>6</v>
       </c>
       <c r="C103" t="s">
-        <v>23</v>
+        <v>144</v>
       </c>
       <c r="D103">
         <v>0.4</v>
       </c>
       <c r="E103" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F103">
         <v>0.7533333333333333</v>
       </c>
       <c r="G103" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -3288,19 +3288,19 @@
         <v>6</v>
       </c>
       <c r="C104" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="D104">
         <v>1</v>
       </c>
       <c r="E104" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F104">
         <v>0.94753761969904249</v>
       </c>
       <c r="G104" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -3311,19 +3311,19 @@
         <v>6</v>
       </c>
       <c r="C105" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="D105">
         <v>1</v>
       </c>
       <c r="E105" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F105">
         <v>0.45333333333333331</v>
       </c>
       <c r="G105" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -3334,19 +3334,19 @@
         <v>6</v>
       </c>
       <c r="C106" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="D106">
         <v>1</v>
       </c>
       <c r="E106" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F106">
         <v>0.63666666666666671</v>
       </c>
       <c r="G106" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -3357,19 +3357,19 @@
         <v>6</v>
       </c>
       <c r="C107" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="D107">
         <v>0.1</v>
       </c>
       <c r="E107" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F107">
         <v>0.95339261285909715</v>
       </c>
       <c r="G107" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -3380,19 +3380,19 @@
         <v>6</v>
       </c>
       <c r="C108" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="D108">
         <v>0.1</v>
       </c>
       <c r="E108" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F108">
         <v>0.45333333333333331</v>
       </c>
       <c r="G108" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -3403,19 +3403,19 @@
         <v>6</v>
       </c>
       <c r="C109" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="D109">
         <v>0.1</v>
       </c>
       <c r="E109" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F109">
         <v>0.7533333333333333</v>
       </c>
       <c r="G109" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -3426,19 +3426,19 @@
         <v>6</v>
       </c>
       <c r="C110" t="s">
-        <v>17</v>
+        <v>152</v>
       </c>
       <c r="D110">
         <v>0.9</v>
       </c>
       <c r="E110" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F110">
         <v>0.93355677154582772</v>
       </c>
       <c r="G110" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -3449,19 +3449,19 @@
         <v>6</v>
       </c>
       <c r="C111" t="s">
-        <v>17</v>
+        <v>152</v>
       </c>
       <c r="D111">
         <v>0.9</v>
       </c>
       <c r="E111" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F111">
         <v>0.11</v>
       </c>
       <c r="G111" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -3472,19 +3472,19 @@
         <v>6</v>
       </c>
       <c r="C112" t="s">
-        <v>17</v>
+        <v>152</v>
       </c>
       <c r="D112">
         <v>0.9</v>
       </c>
       <c r="E112" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F112">
         <v>0.21666666666666659</v>
       </c>
       <c r="G112" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -3495,19 +3495,19 @@
         <v>6</v>
       </c>
       <c r="C113" t="s">
-        <v>16</v>
+        <v>151</v>
       </c>
       <c r="D113">
         <v>1</v>
       </c>
       <c r="E113" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F113">
         <v>0.94402188782489738</v>
       </c>
       <c r="G113" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -3518,19 +3518,19 @@
         <v>6</v>
       </c>
       <c r="C114" t="s">
-        <v>16</v>
+        <v>151</v>
       </c>
       <c r="D114">
         <v>1</v>
       </c>
       <c r="E114" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F114">
         <v>0.64</v>
       </c>
       <c r="G114" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -3541,19 +3541,19 @@
         <v>6</v>
       </c>
       <c r="C115" t="s">
-        <v>16</v>
+        <v>151</v>
       </c>
       <c r="D115">
         <v>1</v>
       </c>
       <c r="E115" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F115">
         <v>0.5971428571428572</v>
       </c>
       <c r="G115" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -3564,19 +3564,19 @@
         <v>8</v>
       </c>
       <c r="C116" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
       <c r="D116" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E116" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F116">
         <v>0.95570451436388504</v>
       </c>
       <c r="G116" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -3587,19 +3587,19 @@
         <v>8</v>
       </c>
       <c r="C117" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
       <c r="D117" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E117" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F117">
         <v>0.59666666666666668</v>
       </c>
       <c r="G117" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -3610,19 +3610,19 @@
         <v>8</v>
       </c>
       <c r="C118" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
       <c r="D118" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E118" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F118">
         <v>0.69261904761904758</v>
       </c>
       <c r="G118" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -3633,19 +3633,19 @@
         <v>8</v>
       </c>
       <c r="C119" t="s">
-        <v>12</v>
+        <v>143</v>
       </c>
       <c r="D119" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E119" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F119">
         <v>0.95801641586867292</v>
       </c>
       <c r="G119" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -3656,19 +3656,19 @@
         <v>8</v>
       </c>
       <c r="C120" t="s">
-        <v>12</v>
+        <v>143</v>
       </c>
       <c r="D120" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E120" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F120">
         <v>0.84000000000000008</v>
       </c>
       <c r="G120" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -3679,19 +3679,19 @@
         <v>8</v>
       </c>
       <c r="C121" t="s">
-        <v>12</v>
+        <v>143</v>
       </c>
       <c r="D121" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E121" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F121">
         <v>0.66731601731601731</v>
       </c>
       <c r="G121" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -3702,19 +3702,19 @@
         <v>8</v>
       </c>
       <c r="C122" t="s">
-        <v>15</v>
+        <v>150</v>
       </c>
       <c r="D122" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="E122" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F122">
         <v>0.96504787961696292</v>
       </c>
       <c r="G122" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -3725,19 +3725,19 @@
         <v>8</v>
       </c>
       <c r="C123" t="s">
-        <v>15</v>
+        <v>150</v>
       </c>
       <c r="D123" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="E123" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F123">
         <v>0.67666666666666664</v>
       </c>
       <c r="G123" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -3748,19 +3748,19 @@
         <v>8</v>
       </c>
       <c r="C124" t="s">
-        <v>15</v>
+        <v>150</v>
       </c>
       <c r="D124" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="E124" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F124">
         <v>0.78119047619047621</v>
       </c>
       <c r="G124" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -3771,19 +3771,19 @@
         <v>8</v>
       </c>
       <c r="C125" t="s">
-        <v>13</v>
+        <v>148</v>
       </c>
       <c r="D125" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="E125" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F125">
         <v>0.95570451436388504</v>
       </c>
       <c r="G125" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -3794,19 +3794,19 @@
         <v>8</v>
       </c>
       <c r="C126" t="s">
-        <v>13</v>
+        <v>148</v>
       </c>
       <c r="D126" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="E126" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F126">
         <v>0.87666666666666671</v>
       </c>
       <c r="G126" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -3817,19 +3817,19 @@
         <v>8</v>
       </c>
       <c r="C127" t="s">
-        <v>13</v>
+        <v>148</v>
       </c>
       <c r="D127" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="E127" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F127">
         <v>0.62882756132756124</v>
       </c>
       <c r="G127" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -3840,19 +3840,19 @@
         <v>8</v>
       </c>
       <c r="C128" t="s">
-        <v>20</v>
+        <v>155</v>
       </c>
       <c r="D128" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="E128" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F128">
         <v>0.95221614227086193</v>
       </c>
       <c r="G128" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -3863,19 +3863,19 @@
         <v>8</v>
       </c>
       <c r="C129" t="s">
-        <v>20</v>
+        <v>155</v>
       </c>
       <c r="D129" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="E129" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F129">
         <v>0.32666666666666672</v>
       </c>
       <c r="G129" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -3886,19 +3886,19 @@
         <v>8</v>
       </c>
       <c r="C130" t="s">
-        <v>20</v>
+        <v>155</v>
       </c>
       <c r="D130" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="E130" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F130">
         <v>0.55666666666666664</v>
       </c>
       <c r="G130" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -3909,19 +3909,19 @@
         <v>8</v>
       </c>
       <c r="C131" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="D131" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="E131" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F131">
         <v>0.96154582763337881</v>
       </c>
       <c r="G131" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -3932,19 +3932,19 @@
         <v>8</v>
       </c>
       <c r="C132" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="D132" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="E132" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F132">
         <v>0.87666666666666659</v>
       </c>
       <c r="G132" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -3955,19 +3955,19 @@
         <v>8</v>
       </c>
       <c r="C133" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="D133" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="E133" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F133">
         <v>0.68313492063492054</v>
       </c>
       <c r="G133" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
@@ -3978,19 +3978,19 @@
         <v>8</v>
       </c>
       <c r="C134" t="s">
-        <v>17</v>
+        <v>152</v>
       </c>
       <c r="D134" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="E134" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F134">
         <v>0.96621067031463748</v>
       </c>
       <c r="G134" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
@@ -4001,19 +4001,19 @@
         <v>8</v>
       </c>
       <c r="C135" t="s">
-        <v>17</v>
+        <v>152</v>
       </c>
       <c r="D135" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="E135" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F135">
         <v>0.62666666666666671</v>
       </c>
       <c r="G135" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
@@ -4024,19 +4024,19 @@
         <v>8</v>
       </c>
       <c r="C136" t="s">
-        <v>17</v>
+        <v>152</v>
       </c>
       <c r="D136" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="E136" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F136">
         <v>0.73833333333333329</v>
       </c>
       <c r="G136" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -4047,19 +4047,19 @@
         <v>8</v>
       </c>
       <c r="C137" t="s">
-        <v>16</v>
+        <v>151</v>
       </c>
       <c r="D137" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="E137" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F137">
         <v>0.95570451436388504</v>
       </c>
       <c r="G137" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -4070,19 +4070,19 @@
         <v>8</v>
       </c>
       <c r="C138" t="s">
-        <v>16</v>
+        <v>151</v>
       </c>
       <c r="D138" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="E138" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F138">
         <v>0.66999999999999993</v>
       </c>
       <c r="G138" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -4093,19 +4093,19 @@
         <v>8</v>
       </c>
       <c r="C139" t="s">
-        <v>16</v>
+        <v>151</v>
       </c>
       <c r="D139" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="E139" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F139">
         <v>0.67154761904761906</v>
       </c>
       <c r="G139" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
@@ -4116,19 +4116,19 @@
         <v>8</v>
       </c>
       <c r="C140" t="s">
-        <v>21</v>
+        <v>156</v>
       </c>
       <c r="D140" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="E140" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F140">
         <v>0.96621067031463748</v>
       </c>
       <c r="G140" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
@@ -4139,19 +4139,19 @@
         <v>8</v>
       </c>
       <c r="C141" t="s">
-        <v>21</v>
+        <v>156</v>
       </c>
       <c r="D141" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="E141" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F141">
         <v>0.76999999999999991</v>
       </c>
       <c r="G141" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
@@ -4162,19 +4162,19 @@
         <v>8</v>
       </c>
       <c r="C142" t="s">
-        <v>21</v>
+        <v>156</v>
       </c>
       <c r="D142" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="E142" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F142">
         <v>0.74821428571428572</v>
       </c>
       <c r="G142" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
@@ -4185,19 +4185,19 @@
         <v>8</v>
       </c>
       <c r="C143" t="s">
-        <v>19</v>
+        <v>154</v>
       </c>
       <c r="D143" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="E143" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F143">
         <v>0.96154582763337881</v>
       </c>
       <c r="G143" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
@@ -4208,19 +4208,19 @@
         <v>8</v>
       </c>
       <c r="C144" t="s">
-        <v>19</v>
+        <v>154</v>
       </c>
       <c r="D144" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="E144" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F144">
         <v>0.87666666666666659</v>
       </c>
       <c r="G144" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
@@ -4231,19 +4231,19 @@
         <v>8</v>
       </c>
       <c r="C145" t="s">
-        <v>19</v>
+        <v>154</v>
       </c>
       <c r="D145" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="E145" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F145">
         <v>0.68313492063492054</v>
       </c>
       <c r="G145" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
@@ -4254,19 +4254,19 @@
         <v>8</v>
       </c>
       <c r="C146" t="s">
-        <v>22</v>
+        <v>146</v>
       </c>
       <c r="D146" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="E146" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F146">
         <v>0.93823529411764706</v>
       </c>
       <c r="G146" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
@@ -4277,19 +4277,19 @@
         <v>8</v>
       </c>
       <c r="C147" t="s">
-        <v>22</v>
+        <v>146</v>
       </c>
       <c r="D147" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="E147" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F147">
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="G147" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
@@ -4300,19 +4300,19 @@
         <v>8</v>
       </c>
       <c r="C148" t="s">
-        <v>22</v>
+        <v>146</v>
       </c>
       <c r="D148" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="E148" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F148">
         <v>0.1</v>
       </c>
       <c r="G148" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
@@ -4323,19 +4323,19 @@
         <v>8</v>
       </c>
       <c r="C149" t="s">
-        <v>23</v>
+        <v>144</v>
       </c>
       <c r="D149" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E149" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F149">
         <v>0.93590971272229828</v>
       </c>
       <c r="G149" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
@@ -4346,19 +4346,19 @@
         <v>8</v>
       </c>
       <c r="C150" t="s">
-        <v>23</v>
+        <v>144</v>
       </c>
       <c r="D150" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E150" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F150">
         <v>0</v>
       </c>
       <c r="G150" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
@@ -4369,19 +4369,19 @@
         <v>8</v>
       </c>
       <c r="C151" t="s">
-        <v>23</v>
+        <v>144</v>
       </c>
       <c r="D151" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E151" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F151">
         <v>0</v>
       </c>
       <c r="G151" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
@@ -4392,19 +4392,19 @@
         <v>8</v>
       </c>
       <c r="C152" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="D152" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="E152" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F152">
         <v>0.95571819425444604</v>
       </c>
       <c r="G152" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
@@ -4415,19 +4415,19 @@
         <v>8</v>
       </c>
       <c r="C153" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="D153" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="E153" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F153">
         <v>0.45333333333333331</v>
       </c>
       <c r="G153" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
@@ -4438,19 +4438,19 @@
         <v>8</v>
       </c>
       <c r="C154" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="D154" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="E154" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F154">
         <v>0.80333333333333334</v>
       </c>
       <c r="G154" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
@@ -4461,19 +4461,19 @@
         <v>8</v>
       </c>
       <c r="C155" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="D155" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E155" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F155">
         <v>0.95339261285909715</v>
       </c>
       <c r="G155" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
@@ -4484,19 +4484,19 @@
         <v>8</v>
       </c>
       <c r="C156" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="D156" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E156" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F156">
         <v>0.41666666666666669</v>
       </c>
       <c r="G156" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
@@ -4507,19 +4507,19 @@
         <v>8</v>
       </c>
       <c r="C157" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="D157" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E157" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F157">
         <v>0.80333333333333334</v>
       </c>
       <c r="G157" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
@@ -4530,19 +4530,19 @@
         <v>7</v>
       </c>
       <c r="C158" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="D158" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E158" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F158">
         <v>0.95339261285909715</v>
       </c>
       <c r="G158" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
@@ -4553,19 +4553,19 @@
         <v>7</v>
       </c>
       <c r="C159" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="D159" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E159" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F159">
         <v>0.45333333333333331</v>
       </c>
       <c r="G159" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
@@ -4576,19 +4576,19 @@
         <v>7</v>
       </c>
       <c r="C160" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="D160" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E160" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F160">
         <v>0.7533333333333333</v>
       </c>
       <c r="G160" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
@@ -4599,19 +4599,19 @@
         <v>7</v>
       </c>
       <c r="C161" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="D161" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="E161" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F161">
         <v>0.95339261285909715</v>
       </c>
       <c r="G161" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
@@ -4622,19 +4622,19 @@
         <v>7</v>
       </c>
       <c r="C162" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="D162" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="E162" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F162">
         <v>0.45333333333333331</v>
       </c>
       <c r="G162" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
@@ -4645,19 +4645,19 @@
         <v>7</v>
       </c>
       <c r="C163" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="D163" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="E163" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F163">
         <v>0.7533333333333333</v>
       </c>
       <c r="G163" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
@@ -4668,19 +4668,19 @@
         <v>7</v>
       </c>
       <c r="C164" t="s">
-        <v>22</v>
+        <v>146</v>
       </c>
       <c r="D164" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E164" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F164">
         <v>0.95339261285909715</v>
       </c>
       <c r="G164" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
@@ -4691,19 +4691,19 @@
         <v>7</v>
       </c>
       <c r="C165" t="s">
-        <v>22</v>
+        <v>146</v>
       </c>
       <c r="D165" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E165" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F165">
         <v>0.45333333333333331</v>
       </c>
       <c r="G165" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
@@ -4714,19 +4714,19 @@
         <v>7</v>
       </c>
       <c r="C166" t="s">
-        <v>22</v>
+        <v>146</v>
       </c>
       <c r="D166" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E166" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F166">
         <v>0.7533333333333333</v>
       </c>
       <c r="G166" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
@@ -4737,19 +4737,19 @@
         <v>7</v>
       </c>
       <c r="C167" t="s">
-        <v>23</v>
+        <v>144</v>
       </c>
       <c r="D167" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E167" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F167">
         <v>0.94060191518467851</v>
       </c>
       <c r="G167" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
@@ -4760,19 +4760,19 @@
         <v>7</v>
       </c>
       <c r="C168" t="s">
-        <v>23</v>
+        <v>144</v>
       </c>
       <c r="D168" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E168" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F168">
         <v>0.47333333333333327</v>
       </c>
       <c r="G168" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
@@ -4783,22 +4783,23 @@
         <v>7</v>
       </c>
       <c r="C169" t="s">
-        <v>23</v>
+        <v>144</v>
       </c>
       <c r="D169" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E169" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F169">
         <v>0.72098039215686271</v>
       </c>
       <c r="G169" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G169" xr:uid="{6FD61CB4-F6C1-4059-931D-DC01F2917455}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G157">
     <sortCondition descending="1" ref="A1"/>
   </sortState>

</xml_diff>